<commit_message>
Added plot to compare measured to simulated pressure potential w.r.t. changing L, theta_s and Ks
</commit_message>
<xml_diff>
--- a/HYDRUS output and Cluster Analysis/Soil properties grouped by cluster.xlsx
+++ b/HYDRUS output and Cluster Analysis/Soil properties grouped by cluster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\Norway\Norway-version-control\HYDRUS output and Cluster Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D6AE5B-F8F0-4290-8F76-851296427083}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704AD311-D2CC-4062-BA93-7D3E078DF324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="193">
   <si>
     <t>SKU 2016</t>
   </si>
@@ -592,9 +592,6 @@
     <t>WC(0.33 kPa)</t>
   </si>
   <si>
-    <t xml:space="preserve">tension table points </t>
-  </si>
-  <si>
     <t>WC (0.01 kPa)</t>
   </si>
   <si>
@@ -602,6 +599,12 @@
   </si>
   <si>
     <t>WC(0.1 kPa)</t>
+  </si>
+  <si>
+    <t>WC (0.03 kPa)</t>
+  </si>
+  <si>
+    <t>WC (0.1 kPa)</t>
   </si>
 </sst>
 </file>
@@ -691,7 +694,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -700,6 +703,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -983,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ133"/>
+  <dimension ref="A1:AM133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AG17" sqref="AG17"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,17 +1001,20 @@
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" customWidth="1"/>
-    <col min="18" max="18" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1057,22 +1064,29 @@
         <v>41</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="Z1" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AE1" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1122,14 +1136,23 @@
         <f>IF(E2=4,"HH",IF(E2=1, "LL", IF(E2=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="2">
+        <v>0.43280000000000002</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.38462839999999998</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.36624390000000001</v>
+      </c>
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>4.0941293857535102E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1179,60 +1202,69 @@
         <f>IF(E3=4,"HH",IF(E3=1, "LL", IF(E3=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q3">
-        <f>Q2+1</f>
+      <c r="Q3" s="2">
+        <v>0.45840360000000002</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.44227939999999999</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.42761189999999999</v>
+      </c>
+      <c r="T3">
+        <f>T2+1</f>
         <v>2</v>
       </c>
-      <c r="R3">
+      <c r="U3">
         <v>3.4874083268607199E-2</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1282,61 +1314,82 @@
         <f>IF(E4=4,"HH",IF(E4=1, "LL", IF(E4=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q4">
-        <f t="shared" ref="Q4:Q39" si="0">Q3+1</f>
+      <c r="Q4" s="2">
+        <v>0.39571519999999999</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.36537560000000002</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.356987</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T39" si="0">T3+1</f>
         <v>3</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>4.3061936183257897E-2</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>143</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>132</v>
       </c>
-      <c r="W4">
+      <c r="Y4" s="2">
         <f>AVERAGE(F3:F4,F6:F7,F11,F13:F14,F20:F21,F24:F26,F29,F33,F35,F39)</f>
         <v>22.71280625</v>
       </c>
-      <c r="X4">
+      <c r="Z4" s="2">
         <f>AVERAGE(G3:G4,G6:G7,G11,G13:G14,G20:G21,G24:G26,G29,G33,G35,G39)</f>
         <v>51.682468749999998</v>
       </c>
-      <c r="Y4">
+      <c r="AA4" s="2">
         <f>AVERAGE(H3:H4,H6:H7,H11,H13:H14,H20:H21,H24:H26,H29,H33,H35,H39)</f>
         <v>25.604743750000001</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="AB4" s="8">
         <f>AVERAGE(I3:I4,I6:I7,I11,I13:I14,I20:I21,I24:I26,I29,I33,I35,I39)</f>
         <v>1.4447062823944283</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AC4" s="8">
         <f>AVERAGE(J3:J4,J6:J7,J11,J13:J14,J20:J21,J24:J26,J29,J33,J35,J39)</f>
         <v>1.6180624999999997</v>
       </c>
-      <c r="AB4" s="6">
+      <c r="AD4" s="8">
         <f>AVERAGE(K3:K4,K6:K7,K11,K13:K14,K20:K21,K24:K26,K29,K33,K35,K39)</f>
         <v>0.15387500000000001</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AE4" s="8">
         <f>AVERAGE(L3:L4,L6:L7,L11,L13:L14,L20:L21,L24:L26,L29,L33,L35,L39)</f>
         <v>9.9496875000000014</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="AF4" s="8">
         <f>AVERAGE(M3:M4,M6:M7,M11,M13:M14,M20:M21,M24:M26,M29,M33,M35,M39)</f>
         <v>0.45482781796436661</v>
       </c>
-      <c r="AE4" s="6">
+      <c r="AG4" s="8">
         <f>AVERAGE(N3:N4,N6:N7,N11,N13:N14,N20:N21,N24:N26,N29,N33,N35,N39)</f>
         <v>0.65950736526007936</v>
       </c>
-      <c r="AF4" s="6">
+      <c r="AH4" s="8">
         <f>AVERAGE(O3:O4,O6:O7,O11,O13:O14,O20:O21,O24:O26,O29,O33,O35,O39)</f>
         <v>-23.59375</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI4" s="2">
+        <f>AVERAGE(Q3:Q4,Q6:Q7,Q11,Q13:Q14,Q20:Q21,Q24:Q26,Q29,Q33,Q35,Q39)</f>
+        <v>0.43237699374999994</v>
+      </c>
+      <c r="AJ4" s="2">
+        <f>AVERAGE(R3:R4,R6:R7,R11,R13:R14,R20:R21,R24:R26,R29,R33,R35,R39)</f>
+        <v>0.40378575</v>
+      </c>
+      <c r="AK4" s="2">
+        <f>AVERAGE(S3:S4,S6:S7,S11,S13:S14,S20:S21,S24:S26,S29,S33,S35,S39)</f>
+        <v>0.38891467500000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1386,61 +1439,82 @@
         <f>IF(E5=4,"HH",IF(E5=1, "LL", IF(E5=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="2">
+        <v>0.35775709999999999</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.3384683</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.33384710000000001</v>
+      </c>
+      <c r="T5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>4.2880768131697201E-2</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>134</v>
       </c>
-      <c r="W5">
+      <c r="Y5" s="2">
         <f>AVERAGE(F12,F17)</f>
         <v>18.841249999999999</v>
       </c>
-      <c r="X5">
+      <c r="Z5" s="2">
         <f>AVERAGE(G12,G17)</f>
         <v>51.537700000000001</v>
       </c>
-      <c r="Y5">
+      <c r="AA5" s="2">
         <f>AVERAGE(H12,H17)</f>
         <v>29.62105</v>
       </c>
-      <c r="Z5">
+      <c r="AB5" s="2">
         <f>AVERAGE(I12,I17)</f>
         <v>1.59623257482575</v>
       </c>
-      <c r="AA5">
+      <c r="AC5" s="2">
         <f>AVERAGE(J12,J17)</f>
         <v>0.23299999999999998</v>
       </c>
-      <c r="AB5">
+      <c r="AD5" s="2">
         <f>AVERAGE(K12,K17)</f>
         <v>0.05</v>
       </c>
-      <c r="AC5">
+      <c r="AE5" s="2">
         <f>AVERAGE(L12,L17)</f>
         <v>4.7095000000000002</v>
       </c>
-      <c r="AD5">
+      <c r="AF5" s="2">
         <f>AVERAGE(M12,M17)</f>
         <v>0.39764808497141552</v>
       </c>
-      <c r="AE5">
+      <c r="AG5" s="2">
         <f>AVERAGE(N12,N17)</f>
         <v>0.86338751312232453</v>
       </c>
-      <c r="AF5">
+      <c r="AH5" s="2">
         <f>AVERAGE(O12,O17)</f>
         <v>-76.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI5" s="2">
+        <f>AVERAGE(Q12,Q17)</f>
+        <v>0.39832239999999997</v>
+      </c>
+      <c r="AJ5" s="2">
+        <f>AVERAGE(R12,R17)</f>
+        <v>0.37576865000000004</v>
+      </c>
+      <c r="AK5" s="2">
+        <f>AVERAGE(S12,S17)</f>
+        <v>0.36763124999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1490,61 +1564,82 @@
         <f>IF(E6=4,"HH",IF(E6=1, "LL", IF(E6=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="2">
+        <v>0.47893819999999998</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.42996289999999998</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.40851419999999999</v>
+      </c>
+      <c r="T6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R6">
+      <c r="U6">
         <v>6.4016025648760702E-2</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>147</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>133</v>
       </c>
-      <c r="W6">
+      <c r="Y6" s="2">
         <f>AVERAGE(F2,F5,F8:F10,F15:F16,F18:F19,F22:F23,F27:F28,F30:F32,F34,F36:F38)</f>
         <v>20.665270000000003</v>
       </c>
-      <c r="X6">
+      <c r="Z6" s="2">
         <f>AVERAGE(G2,G5,G8:G10,G15:G16,G18:G19,G22:G23,G27:G28,G30:G32,G34,G36:G38)</f>
         <v>53.651245000000003</v>
       </c>
-      <c r="Y6">
+      <c r="AA6" s="2">
         <f>AVERAGE(H2,H5,H8:H10,H15:H16,H18:H19,H22:H23,H27:H28,H30:H32,H34,H36:H38)</f>
         <v>25.683505000000004</v>
       </c>
-      <c r="Z6">
+      <c r="AB6" s="2">
         <f>AVERAGE(I2,I5,I8:I10,I15:I16,I18:I19,I22:I23,I27:I28,I30:I32,I34,I36:I38)</f>
         <v>1.6256905034691822</v>
       </c>
-      <c r="AA6">
+      <c r="AC6" s="2">
         <f>AVERAGE(J2,J5,J8:J10,J15:J16,J18:J19,J22:J23,J27:J28,J30:J32,J34,J36:J38)</f>
         <v>0.55630000000000002</v>
       </c>
-      <c r="AB6">
+      <c r="AD6" s="2">
         <f>AVERAGE(K2,K5,K8:K10,K15:K16,K18:K19,K22:K23,K27:K28,K30:K32,K34,K36:K38)</f>
         <v>7.3499999999999996E-2</v>
       </c>
-      <c r="AC6">
+      <c r="AE6" s="2">
         <f>AVERAGE(L2,L5,L8:L10,L15:L16,L18:L19,L22:L23,L27:L28,L30:L32,L34,L36:L38)</f>
         <v>6.1454500000000003</v>
       </c>
-      <c r="AD6">
+      <c r="AF6" s="2">
         <f>AVERAGE(M2,M5,M8:M10,M15:M16,M18:M19,M22:M23,M27:M28,M30:M32,M34,M36:M38)</f>
         <v>0.38653188548332751</v>
       </c>
-      <c r="AE6">
+      <c r="AG6" s="2">
         <f>AVERAGE(N2,N5,N8:N10,N15:N16,N18:N19,N22:N23,N27:N28,N30:N32,N34,N36:N38)</f>
         <v>0.76477724738919972</v>
       </c>
-      <c r="AF6">
+      <c r="AH6" s="2">
         <f>AVERAGE(O2,O5,O8:O10,O15:O16,O18:O19,O22:O23,O27:O28,O30:O32,O34,O36:O38)</f>
         <v>-49.65</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI6" s="2">
+        <f>AVERAGE(Q2,Q5,Q8:Q10,Q15:Q16,Q18:Q19,Q22:Q23,Q27:Q28,Q30:Q32,Q34,Q36:Q38)</f>
+        <v>0.38276169500000001</v>
+      </c>
+      <c r="AJ6" s="2">
+        <f>AVERAGE(R2,R5,R8:R10,R15:R16,R18:R19,R22:R23,R27:R28,R30:R32,R34,R36:R38)</f>
+        <v>0.36231624500000004</v>
+      </c>
+      <c r="AK6" s="2">
+        <f>AVERAGE(S2,S5,S8:S10,S15:S16,S18:S19,S22:S23,S27:S28,S30:S32,S34,S36:S38)</f>
+        <v>0.35497638499999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1594,15 +1689,24 @@
         <f>IF(E7=4,"HH",IF(E7=1, "LL", IF(E7=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="2">
+        <v>0.36112899999999998</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.33169359999999998</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.32370680000000002</v>
+      </c>
+      <c r="T7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R7">
+      <c r="U7">
         <v>4.14781422470182E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1652,60 +1756,69 @@
         <f>IF(E8=4,"HH",IF(E8=1, "LL", IF(E8=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="2">
+        <v>0.36647190000000002</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.34708270000000002</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.33969870000000002</v>
+      </c>
+      <c r="T8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>3.01938164178428E-2</v>
       </c>
-      <c r="V8" s="4" t="s">
+      <c r="X8" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AD8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AE8" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AF8" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AG8" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AH8" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AI8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AK8" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AI8" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AL8" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1755,61 +1868,82 @@
         <f>IF(E9=4,"HH",IF(E9=1, "LL", IF(E9=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="2">
+        <v>0.46960030000000003</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.42625089999999999</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.40359669999999997</v>
+      </c>
+      <c r="T9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R9">
+      <c r="U9">
         <v>6.4698729440839695E-2</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
         <v>144</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>132</v>
       </c>
-      <c r="W9">
+      <c r="Y9" s="2">
         <f>AVERAGE(F51:F56,F62,F65:F70,F74:F78,F80,F83,F85:F87,F89:F90,F93,F95:F97,F99,F101:F102,F109,F117,F122:F123,F128:F133)</f>
         <v>25.127633333333332</v>
       </c>
-      <c r="X9">
+      <c r="Z9" s="2">
         <f>AVERAGE(G51:G56,G62,G65:G70,G74:G78,G80,G83,G85:G87,G89:G90,G93,G95:G97,G99,G101:G102,G109,G117,G122:G123,G128:G133)</f>
         <v>50.268066666666677</v>
       </c>
-      <c r="Y9">
+      <c r="AA9" s="2">
         <f>AVERAGE(H51:H56,H62,H65:H70,H74:H78,H80,H83,H85:H87,H89:H90,H93,H95:H97,H99,H101:H102,H109,H117,H122:H123,H128:H133)</f>
         <v>24.604297619047617</v>
       </c>
-      <c r="Z9" s="6">
+      <c r="AB9" s="8">
         <f>AVERAGE(I51:I56,I62,I65:I70,I74:I78,I80,I83,I85:I87,I89:I90,I93,I95:I97,I99,I101:I102,I109,I117,I122:I123,I128:I133)</f>
         <v>1.4617153388359407</v>
       </c>
-      <c r="AA9" s="6">
+      <c r="AC9" s="8">
         <f>AVERAGE(J51:J56,J62,J65:J70,J74:J78,J80,J83,J85:J87,J89:J90,J93,J95:J97,J99,J101:J102,J109,J117,J122:J123,J128:J133)</f>
         <v>1.656166666666667</v>
       </c>
-      <c r="AB9" s="6">
+      <c r="AD9" s="8">
         <f>AVERAGE(K51:K56,K62,K65:K70,K74:K78,K80,K83,K85:K87,K89:K90,K93,K95:K97,K99,K101:K102,K109,K117,K122:K123,K128:K133)</f>
         <v>0.1528809523809524</v>
       </c>
-      <c r="AC9" s="6">
+      <c r="AE9" s="8">
         <f>AVERAGE(L51:L56,L62,L65:L70,L74:L78,L80,L83,L85:L87,L89:L90,L93,L95:L97,L99,L101:L102,L109,L117,L122:L123,L128:L133)</f>
         <v>10.77702053640771</v>
       </c>
-      <c r="AD9" s="6">
+      <c r="AF9" s="8">
         <f>AVERAGE(M51:M56,M62,M65:M70,M74:M78,M80,M83,M85:M87,M89:M90,M93,M95:M97,M99,M101:M102,M109,M117,M122:M123,M128:M133)</f>
         <v>0.44840930609964502</v>
       </c>
-      <c r="AE9" s="6">
+      <c r="AG9" s="8">
         <f>AVERAGE(N51:N56,N62,N65:N70,N74:N78,N80,N83,N85:N87,N89:N90,N93,N95:N97,N99,N101:N102,N109,N117,N122:N123,N128:N133)</f>
         <v>0.70914662546538521</v>
       </c>
-      <c r="AF9" s="6">
+      <c r="AH9" s="8">
         <f>AVERAGE(O51:O56,O62,O65:O70,O74:O78,O80,O83,O85:O87,O89:O90,O93,O95:O97,O99,O101:O102,O109,O117,O122:O123,O128:O133)</f>
         <v>-22.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI9" s="2">
+        <f>AVERAGE(Q51:Q56,Q62,Q65:Q70,Q74:Q78,Q80,Q83,Q85:Q87,Q89:Q90,Q93,Q95:Q97,Q99,Q101:Q102,Q109,Q117,Q122:Q123,Q128:Q133)</f>
+        <v>0.41594315238095236</v>
+      </c>
+      <c r="AJ9" s="2">
+        <f>AVERAGE(R51:R56,R62,R65:R70,R74:R78,R80,R83,R85:R87,R89:R90,R93,R95:R97,R99,R101:R102,R109,R117,R122:R123,R128:R133)</f>
+        <v>0.39261316904761906</v>
+      </c>
+      <c r="AK9" s="2">
+        <f>AVERAGE(S51:S56,S62,S65:S70,S74:S78,S80,S83,S85:S87,S89:S90,S93,S95:S97,S99,S101:S102,S109,S117,S122:S123,S128:S133)</f>
+        <v>0.37740582857142851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1859,51 +1993,69 @@
         <f>IF(E10=4,"HH",IF(E10=1, "LL", IF(E10=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="2">
+        <v>0.34121190000000001</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0.31885910000000001</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.31036999999999998</v>
+      </c>
+      <c r="T10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="R10">
+      <c r="U10">
         <v>4.7124847095827503E-2</v>
       </c>
-      <c r="U10" s="6" t="s">
+      <c r="W10" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>134</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Y10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Z10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AA10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AB10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AC10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AD10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AE10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AF10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1953,61 +2105,82 @@
         <f>IF(E11=4,"HH",IF(E11=1, "LL", IF(E11=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
+        <v>0.43768220000000002</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.40176699999999999</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.38257869999999999</v>
+      </c>
+      <c r="T11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="R11">
+      <c r="U11">
         <v>8.0234911802205197E-2</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" t="s">
         <v>148</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>133</v>
       </c>
-      <c r="W11">
+      <c r="Y11" s="2">
         <f>AVERAGE(F57:F61,F63:F64,F71:F73,F79,F81:F82,F84,F88,F91:F92,F94,F98,F100,F103:F107,F108,F110:F116,F118:F121,F124:F127)</f>
         <v>24.497258536585367</v>
       </c>
-      <c r="X11">
+      <c r="Z11" s="2">
         <f>AVERAGE(G57:G61,G63:G64,G71:G73,G79,G81:G82,G84,G88,G91:G92,G94,G98,G100,G103:G107,G108,G110:G116,G118:G121,G124:G127)</f>
         <v>52.153929268292693</v>
       </c>
-      <c r="Y11">
+      <c r="AA11" s="2">
         <f>AVERAGE(H57:H61,H63:H64,H71:H73,H79,H81:H82,H84,H88,H91:H92,H94,H98,H100,H103:H107,H108,H110:H116,H118:H121,H124:H127)</f>
         <v>23.348812195121951</v>
       </c>
-      <c r="Z11">
+      <c r="AB11" s="2">
         <f>AVERAGE(I57:I61,I63:I64,I71:I73,I79,I81:I82,I84,I88,I91:I92,I94,I98,I100,I103:I107,I108,I110:I116,I118:I121,I124:I127)</f>
         <v>1.6729618882455453</v>
       </c>
-      <c r="AA11">
+      <c r="AC11" s="2">
         <f>AVERAGE(J57:J61,J63:J64,J71:J73,J79,J81:J82,J84,J88,J91:J92,J94,J98,J100,J103:J107,J108,J110:J116,J118:J121,J124:J127)</f>
         <v>0.74968292682926829</v>
       </c>
-      <c r="AB11">
+      <c r="AD11" s="2">
         <f>AVERAGE(K57:K61,K63:K64,K71:K73,K79,K81:K82,K84,K88,K91:K92,K94,K98,K100,K103:K107,K108,K110:K116,K118:K121,K124:K127)</f>
         <v>8.8975609756097571E-2</v>
       </c>
-      <c r="AC11">
+      <c r="AE11" s="2">
         <f>AVERAGE(L57:L61,L63:L64,L71:L73,L79,L81:L82,L84,L88,L91:L92,L94,L98,L100,L103:L107,L108,L110:L116,L118:L121,L124:L127)</f>
         <v>6.8168122698893292</v>
       </c>
-      <c r="AD11">
+      <c r="AF11" s="2">
         <f>AVERAGE(M57:M61,M63:M64,M71:M73,M79,M81:M82,M84,M88,M91:M92,M94,M98,M100,M103:M107,M108,M110:M116,M118:M121,M124:M127)</f>
         <v>0.3686940522620068</v>
       </c>
-      <c r="AE11">
+      <c r="AG11" s="2">
         <f>AVERAGE(N57:N61,N63:N64,N71:N73,N79,N81:N82,N84,N88,N91:N92,N94,N98,N100,N103:N107,N108,N110:N116,N118:N121,N124:N127)</f>
         <v>0.7953859452041071</v>
       </c>
-      <c r="AF11">
+      <c r="AH11" s="2">
         <f>AVERAGE(O57:O61,O63:O64,O71:O73,O79,O81:O82,O84,O88,O91:O92,O94,O98,O100,O103:O107,O108,O110:O116,O118:O121,O124:O127)</f>
         <v>-52.926829268292686</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI11" s="2">
+        <f>AVERAGE(Q57:Q61,Q63:Q64,Q71:Q73,Q79,Q81:Q82,Q84,Q88,Q91:Q92,Q94,Q98,Q100,Q103:Q107,Q108,Q110:Q116,Q118:Q121,Q124:Q127)</f>
+        <v>0.36353729268292678</v>
+      </c>
+      <c r="AJ11" s="2">
+        <f>AVERAGE(R57:R61,R63:R64,R71:R73,R79,R81:R82,R84,R88,R91:R92,R94,R98,R100,R103:R107,R108,R110:R116,R118:R121,R124:R127)</f>
+        <v>0.3515590878048781</v>
+      </c>
+      <c r="AK11" s="2">
+        <f>AVERAGE(S57:S61,S63:S64,S71:S73,S79,S81:S82,S84,S88,S91:S92,S94,S98,S100,S103:S107,S108,S110:S116,S118:S121,S124:S127)</f>
+        <v>0.34432673902439032</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -2057,15 +2230,24 @@
         <f>IF(E12=4,"HH",IF(E12=1, "LL", IF(E12=0, "NS", NA)))</f>
         <v>LL</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="2">
+        <v>0.35489480000000001</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0.33756510000000001</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0.3301309</v>
+      </c>
+      <c r="T12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="R12">
+      <c r="U12">
         <v>2.9215083133753001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -2115,60 +2297,69 @@
         <f>IF(E13=4,"HH",IF(E13=1, "LL", IF(E13=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
+        <v>0.45946680000000001</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0.41164679999999998</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0.3857778</v>
+      </c>
+      <c r="T13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>6.5385303224042707E-2</v>
       </c>
-      <c r="V13" s="4" t="s">
+      <c r="X13" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="W13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="X13" s="5" t="s">
+      <c r="Z13" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="AA13" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="AB13" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="AC13" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AB13" s="5" t="s">
+      <c r="AD13" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AC13" s="5" t="s">
+      <c r="AE13" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="AD13" s="5" t="s">
+      <c r="AF13" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AE13" s="5" t="s">
+      <c r="AG13" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="AF13" s="5" t="s">
+      <c r="AH13" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="AG13" s="5" t="s">
+      <c r="AI13" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ13" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="AH13" s="5" t="s">
+      <c r="AK13" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="AI13" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ13" s="5" t="s">
+      <c r="AL13" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -2218,61 +2409,83 @@
         <f>IF(E14=4,"HH",IF(E14=1, "LL", IF(E14=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="2">
+        <v>0.48232079999999999</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0.43640960000000001</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0.41787439999999998</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R14">
+      <c r="U14">
         <v>7.7213069014245503E-2</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" t="s">
         <v>150</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>132</v>
       </c>
-      <c r="W14">
+      <c r="Y14" s="2">
         <f>AVERAGE(F3:F4,F6:F7,F11,F13:F14,F20:F21,F24:F26,F29,F33,F35,F39,F51:F56,F62,F65:F70,F74,F75:F78,F80,F83,F85:F87,F89:F90,F93,F95:F97,F99,F101:F102,F109,F117,F122:F123,F128:F133)</f>
         <v>24.461474137931024</v>
       </c>
-      <c r="X14">
+      <c r="Z14" s="2">
         <f>AVERAGE(G3:G4,G6:G7,G11,G13:G14,G20:G21,G24:G26,G29,G33,G35,G39,G51:G56,G62,G65:G70,G74,G75:G78,G80,G83,G85:G87,G89:G90,G93,G95:G97,G99,G101:G102,G109,G117,G122:G123,G128:G133)</f>
         <v>50.658246551724154</v>
       </c>
-      <c r="Y14">
+      <c r="AA14" s="2">
         <f>AVERAGE(H3:H4,H6:H7,H11,H13:H14,H20:H21,H24:H26,H29,H33,H35,H39,H51:H56,H62,H65:H70,H74,H75:H78,H80,H83,H85:H87,H89:H90,H93,H95:H97,H99,H101:H102,H109,H117,H122:H123,H128:H133)</f>
         <v>24.880282758620687</v>
       </c>
-      <c r="Z14" s="6">
+      <c r="AB14" s="8">
         <f>AVERAGE(I3:I4,I6:I7,I11,I13:I14,I20:I21,I24:I26,I29,I33,I35,I39,I51:I56,I62,I65:I70,I74,I75:I78,I80,I83,I85:I87,I89:I90,I93,I95:I97,I99,I101:I102,I109,I117,I122:I123,I128:I133)</f>
         <v>1.4570231853348345</v>
       </c>
-      <c r="AA14" s="6">
+      <c r="AC14" s="8">
         <f>AVERAGE(J3:J4,J6:J7,J11,J13:J14,J20:J21,J24:J26,J29,J33,J35,J39,J51:J56,J62,J65:J70,J74,J75:J78,J80,J83,J85:J87,J89:J90,J93,J95:J97,J99,J101:J102,J109,J117,J122:J123,J128:J133)</f>
         <v>1.6456551724137936</v>
       </c>
-      <c r="AB14" s="6">
+      <c r="AD14" s="8">
         <f>AVERAGE(K3:K4,K6:K7,K11,K13:K14,K20:K21,K24:K26,K29,K33,K35,K39,K51:K56,K62,K65:K70,K74,K75:K78,K80,K83,K85:K87,K89:K90,K93,K95:K97,K99,K101:K102,K109,K117,K122:K123,K128:K133)</f>
         <v>0.15315517241379314</v>
       </c>
-      <c r="AC14" s="6">
+      <c r="AE14" s="8">
         <f>AVERAGE(L3:L4,L6:L7,L11,L13:L14,L20:L21,L24:L26,L29,L33,L35,L39,L51:L56,L62,L65:L70,L74,L75:L78,L80,L83,L85:L87,L89:L90,L93,L95:L97,L99,L101:L102,L109,L117,L122:L123,L128:L133)</f>
         <v>10.548790733260756</v>
       </c>
-      <c r="AD14" s="6">
+      <c r="AF14" s="8">
         <f>AVERAGE(M3:M4,M6:M7,M11,M13:M14,M20:M21,M24:M26,M29,M33,M35,M39,M51:M56,M62,M65:M70,M74,M75:M78,M80,M83,M85:M87,M89:M90,M93,M95:M97,M99,M101:M102,M109,M117,M122:M123,M128:M133)</f>
         <v>0.45017993006232676</v>
       </c>
-      <c r="AE14" s="6">
+      <c r="AG14" s="8">
         <f>AVERAGE(N3:N4,N6:N7,N11,N13:N14,N20:N21,N24:N26,N29,N33,N35,N39,N51:N56,N62,N65:N70,N74,N75:N78,N80,N83,N85:N87,N89:N90,N93,N95:N97,N99,N101:N102,N109,N117,N122:N123,N128:N133)</f>
         <v>0.69545303644323186</v>
       </c>
-      <c r="AF14" s="6">
+      <c r="AH14" s="8">
         <f>AVERAGE(O3:O4,O6:O7,O11,O13:O14,O20:O21,O24:O26,O29,O33,O35,O39,O51:O56,O62,O65:O70,O74,O75:O78,O80,O83,O85:O87,O89:O90,O93,O95:O97,O99,O101:O102,O109,O117,O122:O123,O128:O133)</f>
         <v>-22.801724137931036</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI14" s="2">
+        <f>AVERAGE(Q3:Q4,Q6:Q7,Q11,Q13:Q14,Q20:Q21,Q24:Q26,Q29,Q33,Q35,Q39,Q51:Q56,Q62,Q65:Q70,Q74,Q75:Q78,Q80,Q83,Q85:Q87,Q89:Q90,Q93,Q95:Q97,Q99,Q101:Q102,Q109,Q117,Q122:Q123,Q128:Q133)</f>
+        <v>0.42047662586206885</v>
+      </c>
+      <c r="AJ14" s="2">
+        <f>AVERAGE(R3:R4,R6:R7,R11,R13:R14,R20:R21,R24:R26,R29,R33,R35,R39,R51:R56,R62,R65:R70,R74,R75:R78,R80,R83,R85:R87,R89:R90,R93,R95:R97,R99,R101:R102,R109,R117,R122:R123,R128:R133)</f>
+        <v>0.39569526034482749</v>
+      </c>
+      <c r="AK14" s="2">
+        <f>AVERAGE(S3:S4,S6:S7,S11,S13:S14,S20:S21,S24:S26,S29,S33,S35,S39,S51:S56,S62,S65:S70,S74,S75:S78,S80,S83,S85:S87,S89:S90,S93,S95:S97,S99,S101:S102,S109,S117,S122:S123,S128:S133)</f>
+        <v>0.38058068275862073</v>
+      </c>
+      <c r="AM14" s="8"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -2322,51 +2535,69 @@
         <f>IF(E15=4,"HH",IF(E15=1, "LL", IF(E15=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="2">
+        <v>0.38474520000000001</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0.36852059999999998</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0.3621915</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>4.86232987208991E-2</v>
       </c>
-      <c r="U15" t="s">
+      <c r="W15" t="s">
         <v>151</v>
       </c>
-      <c r="V15" t="s">
+      <c r="X15" t="s">
         <v>134</v>
       </c>
-      <c r="W15">
+      <c r="Y15" s="2">
         <v>18.841249999999999</v>
       </c>
-      <c r="X15">
+      <c r="Z15" s="2">
         <v>51.537700000000001</v>
       </c>
-      <c r="Y15">
+      <c r="AA15" s="2">
         <v>29.62105</v>
       </c>
-      <c r="Z15">
+      <c r="AB15" s="2">
         <v>1.59623257482575</v>
       </c>
-      <c r="AA15">
+      <c r="AC15" s="2">
         <v>0.23299999999999998</v>
       </c>
-      <c r="AB15">
+      <c r="AD15" s="2">
         <v>0.05</v>
       </c>
-      <c r="AC15">
+      <c r="AE15" s="2">
         <v>4.7095000000000002</v>
       </c>
-      <c r="AD15">
+      <c r="AF15" s="2">
         <v>0.39764808497141552</v>
       </c>
-      <c r="AE15">
+      <c r="AG15" s="2">
         <v>0.86338751312232453</v>
       </c>
-      <c r="AF15">
-        <v>0.86338751312232453</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AH15" s="2">
+        <v>-76.25</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>0.39832239999999997</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>0.37576865000000004</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>0.36763124999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -2416,61 +2647,82 @@
         <f>IF(E16=4,"HH",IF(E16=1, "LL", IF(E16=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="2">
+        <v>0.41318110000000002</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0.39183289999999998</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.38138490000000003</v>
+      </c>
+      <c r="T16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>4.6711089091740099E-2</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" t="s">
         <v>152</v>
       </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
         <v>133</v>
       </c>
-      <c r="W16">
+      <c r="Y16" s="2">
         <f>AVERAGE(F2,F5,F8:F10,F15:F16,F18:F19,F22:F23,F27:F28,F30:F32,F34,F36:F38,F57:F61,F63:F64,F71:F73,F79,F81:F82,F84,F88,F91:F92,F94,F98,F100,F103:F108,F110:F116,F118:F121,F124:F127)</f>
         <v>23.240868852459016</v>
       </c>
-      <c r="X16">
+      <c r="Z16" s="2">
         <f>AVERAGE(G2,G5,G8:G10,G15:G16,G18:G19,G22:G23,G27:G28,G30:G32,G34,G36:G38,G57:G61,G63:G64,G71:G73,G79,G81:G82,G84,G88,G91:G92,G94,G98,G100,G103:G108,G110:G116,G118:G121,G124:G127)</f>
         <v>52.644852459016406</v>
       </c>
-      <c r="Y16">
+      <c r="AA16" s="2">
         <f>AVERAGE(H2,H5,H8:H10,H15:H16,H18:H19,H22:H23,H27:H28,H30:H32,H34,H36:H38,H57:H61,H63:H64,H71:H73,H79,H81:H82,H84,H88,H91:H92,H94,H98,H100,H103:H108,H110:H116,H118:H121,H124:H127)</f>
         <v>24.114285245901637</v>
       </c>
-      <c r="Z16">
+      <c r="AB16" s="2">
         <f>AVERAGE(I2,I5,I8:I10,I15:I16,I18:I19,I22:I23,I27:I28,I30:I32,I34,I36:I38,I57:I61,I63:I64,I71:I73,I79,I81:I82,I84,I88,I91:I92,I94,I98,I100,I103:I108,I110:I116,I118:I121,I124:I127)</f>
         <v>1.6574630735647702</v>
       </c>
-      <c r="AA16">
+      <c r="AC16" s="2">
         <f>AVERAGE(J2,J5,J8:J10,J15:J16,J18:J19,J22:J23,J27:J28,J30:J32,J34,J36:J38,J57:J61,J63:J64,J71:J73,J79,J81:J82,J84,J88,J91:J92,J94,J98,J100,J103:J108,J110:J116,J118:J121,J124:J127)</f>
         <v>0.68627868852459017</v>
       </c>
-      <c r="AB16">
+      <c r="AD16" s="2">
         <f>AVERAGE(K2,K5,K8:K10,K15:K16,K18:K19,K22:K23,K27:K28,K30:K32,K34,K36:K38,K57:K61,K63:K64,K71:K73,K79,K81:K82,K84,K88,K91:K92,K94,K98,K100,K103:K108,K110:K116,K118:K121,K124:K127)</f>
         <v>8.3901639344262272E-2</v>
       </c>
-      <c r="AC16">
+      <c r="AE16" s="2">
         <f>AVERAGE(L2,L5,L8:L10,L15:L16,L18:L19,L22:L23,L27:L28,L30:L32,L34,L36:L38,L57:L61,L63:L64,L71:L73,L79,L81:L82,L84,L88,L91:L92,L94,L98,L100,L103:L108,L110:L116,L118:L121,L124:L127)</f>
         <v>6.5966934928764358</v>
       </c>
-      <c r="AD16">
+      <c r="AF16" s="2">
         <f>AVERAGE(M2,M5,M8:M10,M15:M16,M18:M19,M22:M23,M27:M28,M30:M32,M34,M36:M38,M57:M61,M63:M64,M71:M73,M79,M81:M82,M84,M88,M91:M92,M94,M98,M100,M103:M108,M110:M116,M118:M121,M124:M127)</f>
         <v>0.37454252217063666</v>
       </c>
-      <c r="AE16">
+      <c r="AG16" s="2">
         <f>AVERAGE(N2,N5,N8:N10,N15:N16,N18:N19,N22:N23,N27:N28,N30:N32,N34,N36:N38,N57:N61,N63:N64,N71:N73,N79,N81:N82,N84,N88,N91:N92,N94,N98,N100,N103:N108,N110:N116,N118:N121,N124:N127)</f>
         <v>0.7853503065762687</v>
       </c>
-      <c r="AF16">
+      <c r="AH16" s="2">
         <f>AVERAGE(O2,O5,O8:O10,O15:O16,O18:O19,O22:O23,O27:O28,O30:O32,O34,O36:O38,O57:O61,O63:O64,O71:O73,O79,O81:O82,O84,O88,O91:O92,O94,O98,O100,O103:O108,O110:O116,O118:O121,O124:O127)</f>
         <v>-51.852459016393439</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI16" s="2">
+        <f>AVERAGE(Q2,Q5,Q8:Q10,Q15:Q16,Q18:Q19,Q22:Q23,Q27:Q28,Q30:Q32,Q34,Q36:Q38,Q57:Q61,Q63:Q64,Q71:Q73,Q79,Q81:Q82,Q84,Q88,Q91:Q92,Q94,Q98,Q100,Q103:Q108,Q110:Q116,Q118:Q121,Q124:Q127)</f>
+        <v>0.36984037540983605</v>
+      </c>
+      <c r="AJ16" s="2">
+        <f>AVERAGE(R2,R5,R8:R10,R15:R16,R18:R19,R22:R23,R27:R28,R30:R32,R34,R36:R38,R57:R61,R63:R64,R71:R73,R79,R81:R82,R84,R88,R91:R92,R94,R98,R100,R103:R108,R110:R116,R118:R121,R124:R127)</f>
+        <v>0.35508602459016403</v>
+      </c>
+      <c r="AK16" s="2">
+        <f>AVERAGE(S2,S5,S8:S10,S15:S16,S18:S19,S22:S23,S27:S28,S30:S32,S34,S36:S38,S57:S61,S63:S64,S71:S73,S79,S81:S82,S84,S88,S91:S92,S94,S98,S100,S103:S108,S110:S116,S118:S121,S124:S127)</f>
+        <v>0.34781842622950798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2520,15 +2772,24 @@
         <f>IF(E17=4,"HH",IF(E17=1, "LL", IF(E17=0, "NS", NA)))</f>
         <v>LL</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="2">
+        <v>0.44174999999999998</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0.41397220000000001</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0.40513159999999998</v>
+      </c>
+      <c r="T17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="R17">
+      <c r="U17">
         <v>5.9012601708938801E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -2578,18 +2839,27 @@
         <f>IF(E18=4,"HH",IF(E18=1, "LL", IF(E18=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="2">
+        <v>0.43019770000000002</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0.3926249</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0.37861040000000001</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="R18">
+      <c r="U18">
         <v>3.5048305249981301E-2</v>
       </c>
-      <c r="V18" s="4" t="s">
+      <c r="X18" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -2639,15 +2909,24 @@
         <f>IF(E19=4,"HH",IF(E19=1, "LL", IF(E19=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="2">
+        <v>0.37167060000000002</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0.34012550000000003</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0.3318374</v>
+      </c>
+      <c r="T19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="R19">
+      <c r="U19">
         <v>2.0481057702669302E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -2697,60 +2976,69 @@
         <f>IF(E20=4,"HH",IF(E20=1, "LL", IF(E20=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="2">
+        <v>0.47001799999999999</v>
+      </c>
+      <c r="R20" s="2">
+        <v>0.44457960000000002</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0.4200468</v>
+      </c>
+      <c r="T20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="R20">
+      <c r="U20">
         <v>3.1307586836428501E-2</v>
       </c>
-      <c r="V20" s="4" t="s">
+      <c r="X20" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="W20" s="3" t="s">
+      <c r="Y20" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="X20" s="3" t="s">
+      <c r="Z20" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="Y20" s="3" t="s">
+      <c r="AA20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="Z20" s="3" t="s">
+      <c r="AB20" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AA20" s="3" t="s">
+      <c r="AC20" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="AB20" s="3" t="s">
+      <c r="AD20" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="AC20" s="3" t="s">
+      <c r="AE20" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AD20" s="3" t="s">
+      <c r="AF20" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="AE20" s="3" t="s">
+      <c r="AG20" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="AF20" s="3" t="s">
+      <c r="AH20" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AG20" s="3" t="s">
+      <c r="AI20" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ20" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AH20" s="3" t="s">
+      <c r="AK20" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AI20" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ20" s="3" t="s">
+      <c r="AL20" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -2800,61 +3088,83 @@
         <f>IF(E21=4,"HH",IF(E21=1, "LL", IF(E21=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="2">
+        <v>0.43299739999999998</v>
+      </c>
+      <c r="R21" s="2">
+        <v>0.39780359999999998</v>
+      </c>
+      <c r="S21" s="2">
+        <v>0.38467269999999998</v>
+      </c>
+      <c r="T21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R21">
+      <c r="U21">
         <v>2.8331596012239502E-2</v>
       </c>
-      <c r="U21" t="s">
+      <c r="W21" t="s">
         <v>143</v>
       </c>
-      <c r="V21" t="s">
+      <c r="X21" t="s">
         <v>132</v>
       </c>
-      <c r="W21">
+      <c r="Y21" s="2">
         <f>STDEV(F3:F4,F6:F7,F11,F13:F14,F20:F21,F24:F26,F29,F33,F35,F39)</f>
         <v>2.75888003181695</v>
       </c>
-      <c r="X21">
+      <c r="Z21" s="2">
         <f>STDEV(G3:G4,G6:G7,G11,G13:G14,G20:G21,G24:G26,G29,G33,G35,G39)</f>
         <v>5.0260795112053618</v>
       </c>
-      <c r="Y21">
+      <c r="AA21" s="2">
         <f>STDEV(H3:H4,H6:H7,H11,H13:H14,H20:H21,H24:H26,H29,H33,H35,H39)</f>
         <v>7.0028727878367878</v>
       </c>
-      <c r="Z21">
+      <c r="AB21" s="2">
         <f>STDEV(I3:I4,I6:I7,I11,I13:I14,I20:I21,I24:I26,I29,I33,I35,I39)</f>
         <v>0.14117305497300736</v>
       </c>
-      <c r="AA21">
+      <c r="AC21" s="2">
         <f>STDEV(J3:J4,J6:J7,J11,J13:J14,J20:J21,J24:J26,J29,J33,J35,J39)</f>
         <v>0.6608013790088525</v>
       </c>
-      <c r="AB21">
+      <c r="AD21" s="2">
         <f>STDEV(K3:K4,K6:K7,K11,K13:K14,K20:K21,K24:K26,K29,K33,K35,K39)</f>
         <v>5.2792518409335187E-2</v>
       </c>
-      <c r="AC21">
+      <c r="AE21" s="2">
         <f>STDEV(L3:L4,L6:L7,L11,L13:L14,L20:L21,L24:L26,L29,L33,L35,L39)</f>
         <v>2.0439001188495709</v>
       </c>
-      <c r="AD21">
+      <c r="AF21" s="2">
         <f>STDEV(M3:M4,M6:M7,M11,M13:M14,M20:M21,M24:M26,M29,M33,M35,M39)</f>
         <v>5.3272850933210075E-2</v>
       </c>
-      <c r="AE21">
+      <c r="AG21" s="2">
         <f>STDEV(N3:N4,N6:N7,N11,N13:N14,N20:N21,N24:N26,N29,N33,N35,N39)</f>
         <v>0.17268950575415823</v>
       </c>
-      <c r="AF21">
+      <c r="AH21" s="2">
         <f>STDEV(O3:O4,O6:O7,O11,O13:O14,O20:O21,O24:O26,O29,O33,O35,O39)</f>
         <v>13.813301258810895</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI21" s="2">
+        <f>STDEV(Q3:Q4,Q6:Q7,Q11,Q13:Q14,Q20:Q21,Q24:Q26,Q29,Q33,Q35,Q39)</f>
+        <v>4.1074426521514482E-2</v>
+      </c>
+      <c r="AJ21" s="2">
+        <f>STDEV(R3:R4,R6:R7,R11,R13:R14,R20:R21,R24:R26,R29,R33,R35,R39)</f>
+        <v>3.8600550232416812E-2</v>
+      </c>
+      <c r="AK21" s="2">
+        <f>STDEV(S3:S4,S6:S7,S11,S13:S14,S20:S21,S24:S26,S29,S33,S35,S39)</f>
+        <v>3.468582639358618E-2</v>
+      </c>
+      <c r="AM21" s="2"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -2904,51 +3214,69 @@
         <f>IF(E22=4,"HH",IF(E22=1, "LL", IF(E22=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="2">
+        <v>0.45542850000000001</v>
+      </c>
+      <c r="R22" s="2">
+        <v>0.42649130000000002</v>
+      </c>
+      <c r="S22" s="2">
+        <v>0.41233140000000001</v>
+      </c>
+      <c r="T22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="R22">
+      <c r="U22">
         <v>7.2328062573785906E-2</v>
       </c>
-      <c r="U22" t="s">
+      <c r="W22" t="s">
         <v>146</v>
       </c>
-      <c r="V22" t="s">
+      <c r="X22" t="s">
         <v>134</v>
       </c>
-      <c r="W22" t="s">
+      <c r="Y22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Z22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="AA22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AB22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AC22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AD22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AE22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AF22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AG22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AH22" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK22" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -2998,61 +3326,82 @@
         <f>IF(E23=4,"HH",IF(E23=1, "LL", IF(E23=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="2">
+        <v>0.3535008</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0.34312789999999999</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0.33925860000000002</v>
+      </c>
+      <c r="T23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="R23">
+      <c r="U23">
         <v>6.5786724447862099E-2</v>
       </c>
-      <c r="U23" t="s">
+      <c r="W23" t="s">
         <v>147</v>
       </c>
-      <c r="V23" t="s">
+      <c r="X23" t="s">
         <v>133</v>
       </c>
-      <c r="W23">
+      <c r="Y23" s="2">
         <f>STDEV(F2,F5,F8:F10,F15:F16,F18:F19,F22:F23,F27:F28,F30:F32,F34,F36:F38)</f>
         <v>4.9024967184937394</v>
       </c>
-      <c r="X23">
+      <c r="Z23" s="2">
         <f>STDEV(G2,G5,G8:G10,G15:G16,G18:G19,G22:G23,G27:G28,G30:G32,G34,G36:G38)</f>
         <v>4.4310028740651575</v>
       </c>
-      <c r="Y23">
+      <c r="AA23" s="2">
         <f>STDEV(H2,H5,H8:H10,H15:H16,H18:H19,H22:H23,H27:H28,H30:H32,H34,H36:H38)</f>
         <v>5.592817999944204</v>
       </c>
-      <c r="Z23">
+      <c r="AB23" s="2">
         <f>STDEV(I2,I5,I8:I10,I15:I16,I18:I19,I22:I23,I27:I28,I30:I32,I34,I36:I38)</f>
         <v>0.15302240724521216</v>
       </c>
-      <c r="AA23">
+      <c r="AC23" s="2">
         <f>STDEV(J2,J5,J8:J10,J15:J16,J18:J19,J22:J23,J27:J28,J30:J32,J34,J36:J38)</f>
         <v>0.63040739542816793</v>
       </c>
-      <c r="AB23">
+      <c r="AD23" s="2">
         <f>STDEV(K2,K5,K8:K10,K15:K16,K18:K19,K22:K23,K27:K28,K30:K32,K34,K36:K38)</f>
         <v>4.7158746467872256E-2</v>
       </c>
-      <c r="AC23">
+      <c r="AE23" s="2">
         <f>STDEV(L2,L5,L8:L10,L15:L16,L18:L19,L22:L23,L27:L28,L30:L32,L34,L36:L38)</f>
         <v>2.8342622817196967</v>
       </c>
-      <c r="AD23">
+      <c r="AF23" s="2">
         <f>STDEV(M2,M5,M8:M10,M15:M16,M18:M19,M22:M23,M27:M28,M30:M32,M34,M36:M38)</f>
         <v>5.7744304620833783E-2</v>
       </c>
-      <c r="AE23">
+      <c r="AG23" s="2">
         <f>STDEV(N2,N5,N8:N10,N15:N16,N18:N19,N22:N23,N27:N28,N30:N32,N34,N36:N38)</f>
         <v>0.16701432116578072</v>
       </c>
-      <c r="AF23">
+      <c r="AH23" s="2">
         <f>STDEV(O2,O5,O8:O10,O15:O16,O18:O19,O22:O23,O27:O28,O30:O32,O34,O36:O38)</f>
         <v>24.143812545050263</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI23" s="2">
+        <f>STDEV(Q2,Q5,Q8:Q10,Q15:Q16,Q18:Q19,Q22:Q23,Q27:Q28,Q30:Q32,Q34,Q36:Q38)</f>
+        <v>4.1188098626583014E-2</v>
+      </c>
+      <c r="AJ23" s="2">
+        <f>STDEV(R2,R5,R8:R10,R15:R16,R18:R19,R22:R23,R27:R28,R30:R32,R34,R36:R38)</f>
+        <v>3.4347695838363168E-2</v>
+      </c>
+      <c r="AK23" s="2">
+        <f>STDEV(S2,S5,S8:S10,S15:S16,S18:S19,S22:S23,S27:S28,S30:S32,S34,S36:S38)</f>
+        <v>3.0926849321197894E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -3102,15 +3451,24 @@
         <f>IF(E24=4,"HH",IF(E24=1, "LL", IF(E24=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="2">
+        <v>0.40787420000000002</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0.38292979999999999</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0.36914039999999998</v>
+      </c>
+      <c r="T24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="R24">
+      <c r="U24">
         <v>4.8284192737828503E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
@@ -3160,60 +3518,69 @@
         <f>IF(E25=4,"HH",IF(E25=1, "LL", IF(E25=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="2">
+        <v>0.44184220000000002</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0.41175250000000002</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.39862170000000002</v>
+      </c>
+      <c r="T25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="R25">
+      <c r="U25">
         <v>3.3774585558073202E-2</v>
       </c>
-      <c r="V25" s="4" t="s">
+      <c r="X25" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="W25" s="1" t="s">
+      <c r="Y25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="X25" s="1" t="s">
+      <c r="Z25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Y25" s="1" t="s">
+      <c r="AA25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Z25" s="1" t="s">
+      <c r="AB25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AA25" s="1" t="s">
+      <c r="AC25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AB25" s="1" t="s">
+      <c r="AD25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AC25" s="1" t="s">
+      <c r="AE25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AD25" s="1" t="s">
+      <c r="AF25" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AE25" s="1" t="s">
+      <c r="AG25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AF25" s="1" t="s">
+      <c r="AH25" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AG25" s="1" t="s">
+      <c r="AI25" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AH25" s="1" t="s">
+      <c r="AK25" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AI25" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ25" s="1" t="s">
+      <c r="AL25" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
@@ -3263,61 +3630,82 @@
         <f>IF(E26=4,"HH",IF(E26=1, "LL", IF(E26=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="2">
+        <v>0.33085589999999998</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0.31167420000000001</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0.30854579999999998</v>
+      </c>
+      <c r="T26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="R26">
+      <c r="U26">
         <v>3.2558012788390003E-2</v>
       </c>
-      <c r="U26" t="s">
+      <c r="W26" t="s">
         <v>144</v>
       </c>
-      <c r="V26" t="s">
+      <c r="X26" t="s">
         <v>132</v>
       </c>
-      <c r="W26">
+      <c r="Y26" s="2">
         <f>STDEV(F51:F56,F62,F65:F70,F74:F78,F80,F83,F85:F87,F89:F90,F93,F95:F97,F99,F101:F102,F109,F117,F122:F123,F128:F133)</f>
         <v>2.6345505866268533</v>
       </c>
-      <c r="X26">
+      <c r="Z26" s="2">
         <f>STDEV(G51:G56,G62,G65:G70,G74:G78,G80,G83,G85:G87,G89:G90,G93,G95:G97,G99,G101:G102,G109,G117,G122:G123,G128:G133)</f>
         <v>4.2328829132635324</v>
       </c>
-      <c r="Y26">
+      <c r="AA26" s="2">
         <f>STDEV(H51:H56,H62,H65:H70,H74:H78,H80,H83,H85:H87,H89:H90,H93,H95:H97,H99,H101:H102,H109,H117,H122:H123,H128:H133)</f>
         <v>5.9445030026923726</v>
       </c>
-      <c r="Z26">
+      <c r="AB26" s="2">
         <f>STDEV(I51:I56,I62,I65:I70,I74:I78,I80,I83,I85:I87,I89:I90,I93,I95:I97,I99,I101:I102,I109,I117,I122:I123,I128:I133)</f>
         <v>0.10757125058395846</v>
       </c>
-      <c r="AA26">
+      <c r="AC26" s="2">
         <f>STDEV(J51:J56,J62,J65:J70,J74:J78,J80,J83,J85:J87,J89:J90,J93,J95:J97,J99,J101:J102,J109,J117,J122:J123,J128:J133)</f>
         <v>0.61598590087866523</v>
       </c>
-      <c r="AB26">
+      <c r="AD26" s="2">
         <f>STDEV(K51:K56,K62,K65:K70,K74:K78,K80,K83,K85:K87,K89:K90,K93,K95:K97,K99,K101:K102,K109,K117,K122:K123,K128:K133)</f>
         <v>5.4644394701026444E-2</v>
       </c>
-      <c r="AC26">
+      <c r="AE26" s="2">
         <f>STDEV(L51:L56,L62,L65:L70,L74:L78,L80,L83,L85:L87,L89:L90,L93,L95:L97,L99,L101:L102,L109,L117,L122:L123,L128:L133)</f>
         <v>1.3531476395679565</v>
       </c>
-      <c r="AD26">
+      <c r="AF26" s="2">
         <f>STDEV(M51:M56,M62,M65:M70,M74:M78,M80,M83,M85:M87,M89:M90,M93,M95:M97,M99,M101:M102,M109,M117,M122:M123,M128:M133)</f>
         <v>4.059292474866371E-2</v>
       </c>
-      <c r="AE26">
+      <c r="AG26" s="2">
         <f>STDEV(N51:N56,N62,N65:N70,N74:N78,N80,N83,N85:N87,N89:N90,N93,N95:N97,N99,N101:N102,N109,N117,N122:N123,N128:N133)</f>
         <v>0.17918478834221402</v>
       </c>
-      <c r="AF26">
+      <c r="AH26" s="2">
         <f>STDEV(O51:O56,O62,O65:O70,O74:O78,O80,O83,O85:O87,O89:O90,O93,O95:O97,O99,O101:O102,O109,O117,O122:O123,O128:O133)</f>
         <v>9.0728756836370081</v>
       </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI26" s="2">
+        <f>STDEV(Q51:Q56,Q62,Q65:Q70,Q74:Q78,Q80,Q83,Q85:Q87,Q89:Q90,Q93,Q95:Q97,Q99,Q101:Q102,Q109,Q117,Q122:Q123,Q128:Q133)</f>
+        <v>3.1536872339890575E-2</v>
+      </c>
+      <c r="AJ26" s="2">
+        <f>STDEV(R51:R56,R62,R65:R70,R74:R78,R80,R83,R85:R87,R89:R90,R93,R95:R97,R99,R101:R102,R109,R117,R122:R123,R128:R133)</f>
+        <v>2.9596465453376707E-2</v>
+      </c>
+      <c r="AK26" s="2">
+        <f>STDEV(S51:S56,S62,S65:S70,S74:S78,S80,S83,S85:S87,S89:S90,S93,S95:S97,S99,S101:S102,S109,S117,S122:S123,S128:S133)</f>
+        <v>2.3310459570981927E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -3367,51 +3755,69 @@
         <f>IF(E27=4,"HH",IF(E27=1, "LL", IF(E27=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="2">
+        <v>0.42042829999999998</v>
+      </c>
+      <c r="R27" s="2">
+        <v>0.40717399999999998</v>
+      </c>
+      <c r="S27" s="2">
+        <v>0.40334589999999998</v>
+      </c>
+      <c r="T27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="R27">
+      <c r="U27">
         <v>3.5160545408587297E-2</v>
       </c>
-      <c r="U27" t="s">
+      <c r="W27" t="s">
         <v>145</v>
       </c>
-      <c r="V27" t="s">
+      <c r="X27" t="s">
         <v>134</v>
       </c>
-      <c r="W27" t="s">
+      <c r="Y27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Z27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="AA27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AB27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AC27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AD27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AE27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AF27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AG27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AF27" t="s">
+      <c r="AH27" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK27" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -3461,61 +3867,82 @@
         <f>IF(E28=4,"HH",IF(E28=1, "LL", IF(E28=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="2">
+        <v>0.32617629999999997</v>
+      </c>
+      <c r="R28" s="2">
+        <v>0.31226340000000002</v>
+      </c>
+      <c r="S28" s="2">
+        <v>0.30905270000000001</v>
+      </c>
+      <c r="T28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="R28">
+      <c r="U28">
         <v>3.7406294326575801E-2</v>
       </c>
-      <c r="U28" t="s">
+      <c r="W28" t="s">
         <v>148</v>
       </c>
-      <c r="V28" t="s">
+      <c r="X28" t="s">
         <v>133</v>
       </c>
-      <c r="W28">
+      <c r="Y28" s="2">
         <f>STDEV(F57:F61,F63:F64,F71:F73,F79,F81:F82,F84,F88,F91:F92,F94,F98,F100,F103:F107,F108,F110:F116,F118:F121,F124:F127)</f>
         <v>4.741787920235133</v>
       </c>
-      <c r="X28">
+      <c r="Z28" s="2">
         <f>STDEV(G57:G61,G63:G64,G71:G73,G79,G81:G82,G84,G88,G91:G92,G94,G98,G100,G103:G107,G108,G110:G116,G118:G121,G124:G127)</f>
         <v>4.978655226175233</v>
       </c>
-      <c r="Y28">
+      <c r="AA28" s="2">
         <f>STDEV(H57:H61,H63:H64,H71:H73,H79,H81:H82,H84,H88,H91:H92,H94,H98,H100,H103:H107,H108,H110:H116,H118:H121,H124:H127)</f>
         <v>6.5737173055735809</v>
       </c>
-      <c r="Z28">
+      <c r="AB28" s="2">
         <f>STDEV(I57:I61,I63:I64,I71:I73,I79,I81:I82,I84,I88,I91:I92,I94,I98,I100,I103:I107,I108,I110:I116,I118:I121,I124:I127)</f>
         <v>0.16707402968960514</v>
       </c>
-      <c r="AA28">
+      <c r="AC28" s="2">
         <f>STDEV(J57:J61,J63:J64,J71:J73,J79,J81:J82,J84,J88,J91:J92,J94,J98,J100,J103:J107,J108,J110:J116,J118:J121,J124:J127)</f>
         <v>0.82341084638910333</v>
       </c>
-      <c r="AB28">
+      <c r="AD28" s="2">
         <f>STDEV(K57:K61,K63:K64,K71:K73,K79,K81:K82,K84,K88,K91:K92,K94,K98,K100,K103:K107,K108,K110:K116,K118:K121,K124:K127)</f>
         <v>7.0599747805809493E-2</v>
       </c>
-      <c r="AC28">
+      <c r="AE28" s="2">
         <f>STDEV(L57:L61,L63:L64,L71:L73,L79,L81:L82,L84,L88,L91:L92,L94,L98,L100,L103:L107,L108,L110:L116,L118:L121,L124:L127)</f>
         <v>2.9334499028974523</v>
       </c>
-      <c r="AD28">
+      <c r="AF28" s="2">
         <f>STDEV(M57:M61,M63:M64,M71:M73,M79,M81:M82,M84,M88,M91:M92,M94,M98,M100,M103:M107,M108,M110:M116,M118:M121,M124:M127)</f>
         <v>6.3046542764163618E-2</v>
       </c>
-      <c r="AE28">
+      <c r="AG28" s="2">
         <f>STDEV(N57:N61,N63:N64,N71:N73,N79,N81:N82,N84,N88,N91:N92,N94,N98,N100,N103:N107,N108,N110:N116,N118:N121,N124:N127)</f>
         <v>0.22723567108516934</v>
       </c>
-      <c r="AF28">
+      <c r="AH28" s="2">
         <f>STDEV(O57:O61,O63:O64,O71:O73,O79,O81:O82,O84,O88,O91:O92,O94,O98,O100,O103:O107,O108,O110:O116,O118:O121,O124:O127)</f>
         <v>21.750735900082137</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI28" s="2">
+        <f>STDEV(Q57:Q61,Q63:Q64,Q71:Q73,Q79,Q81:Q82,Q84,Q88,Q91:Q92,Q94,Q98,Q100,Q103:Q107,Q108,Q110:Q116,Q118:Q121,Q124:Q127)</f>
+        <v>4.9955329579757179E-2</v>
+      </c>
+      <c r="AJ28" s="2">
+        <f>STDEV(R57:R61,R63:R64,R71:R73,R79,R81:R82,R84,R88,R91:R92,R94,R98,R100,R103:R107,R108,R110:R116,R118:R121,R124:R127)</f>
+        <v>4.6438293625105792E-2</v>
+      </c>
+      <c r="AK28" s="2">
+        <f>STDEV(S57:S61,S63:S64,S71:S73,S79,S81:S82,S84,S88,S91:S92,S94,S98,S100,S103:S107,S108,S110:S116,S118:S121,S124:S127)</f>
+        <v>4.2496974994979023E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
@@ -3565,15 +3992,24 @@
         <f>IF(E29=4,"HH",IF(E29=1, "LL", IF(E29=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="2">
+        <v>0.44471060000000001</v>
+      </c>
+      <c r="R29" s="2">
+        <v>0.43219730000000001</v>
+      </c>
+      <c r="S29" s="2">
+        <v>0.423265</v>
+      </c>
+      <c r="T29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="R29">
+      <c r="U29">
         <v>3.1015332771711E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
@@ -3623,60 +4059,69 @@
         <f>IF(E30=4,"HH",IF(E30=1, "LL", IF(E30=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="2">
+        <v>0.39238729999999999</v>
+      </c>
+      <c r="R30" s="2">
+        <v>0.37979160000000001</v>
+      </c>
+      <c r="S30" s="2">
+        <v>0.37246469999999998</v>
+      </c>
+      <c r="T30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="R30">
+      <c r="U30">
         <v>2.32888400205707E-2</v>
       </c>
-      <c r="V30" s="4" t="s">
+      <c r="X30" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="W30" s="5" t="s">
+      <c r="Y30" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="X30" s="5" t="s">
+      <c r="Z30" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="Y30" s="5" t="s">
+      <c r="AA30" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Z30" s="5" t="s">
+      <c r="AB30" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="AA30" s="5" t="s">
+      <c r="AC30" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AB30" s="5" t="s">
+      <c r="AD30" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AC30" s="5" t="s">
+      <c r="AE30" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="AD30" s="5" t="s">
+      <c r="AF30" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AE30" s="5" t="s">
+      <c r="AG30" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="AF30" s="5" t="s">
+      <c r="AH30" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="AG30" s="5" t="s">
+      <c r="AI30" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ30" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="AH30" s="5" t="s">
+      <c r="AK30" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="AI30" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="AJ30" s="5" t="s">
+      <c r="AL30" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
@@ -3726,61 +4171,82 @@
         <f>IF(E31=4,"HH",IF(E31=1, "LL", IF(E31=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="2">
+        <v>0.38265339999999998</v>
+      </c>
+      <c r="R31" s="2">
+        <v>0.37598510000000002</v>
+      </c>
+      <c r="S31" s="2">
+        <v>0.3768495</v>
+      </c>
+      <c r="T31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="R31">
+      <c r="U31">
         <v>3.9103912312776899E-2</v>
       </c>
-      <c r="U31" t="s">
+      <c r="W31" t="s">
         <v>150</v>
       </c>
-      <c r="V31" t="s">
+      <c r="X31" t="s">
         <v>132</v>
       </c>
-      <c r="W31">
+      <c r="Y31" s="2">
         <f>STDEV(F3:F4,F6:F7,F11,F13:F14,F20:F21,F24:F26,F29,F33,F35,F39,F51:F56,F62,F65:F70,F74,F75:F78,F80,F83,F85:F87,F89:F90,F93,F95:F97,F99,F101:F102,F109,F117,F122:F123,F128:F133)</f>
         <v>2.8602235932449704</v>
       </c>
-      <c r="X31">
+      <c r="Z31" s="2">
         <f>STDEV(G3:G4,G6:G7,G11,G13:G14,G20:G21,G24:G26,G29,G33,G35,G39,G51:G56,G62,G65:G70,G74,G75:G78,G80,G83,G85:G87,G89:G90,G93,G95:G97,G99,G101:G102,G109,G117,G122:G123,G128:G133)</f>
         <v>4.4656779391898436</v>
       </c>
-      <c r="Y31">
+      <c r="AA31" s="2">
         <f>STDEV(H3:H4,H6:H7,H11,H13:H14,H20:H21,H24:H26,H29,H33,H35,H39,H51:H56,H62,H65:H70,H74,H75:H78,H80,H83,H85:H87,H89:H90,H93,H95:H97,H99,H101:H102,H109,H117,H122:H123,H128:H133)</f>
         <v>6.2069877292956974</v>
       </c>
-      <c r="Z31">
+      <c r="AB31" s="2">
         <f>STDEV(I3:I4,I6:I7,I11,I13:I14,I20:I21,I24:I26,I29,I33,I35,I39,I51:I56,I62,I65:I70,I74,I75:I78,I80,I83,I85:I87,I89:I90,I93,I95:I97,I99,I101:I102,I109,I117,I122:I123,I128:I133)</f>
         <v>0.11673436528191748</v>
       </c>
-      <c r="AA31">
+      <c r="AC31" s="2">
         <f>STDEV(J3:J4,J6:J7,J11,J13:J14,J20:J21,J24:J26,J29,J33,J35,J39,J51:J56,J62,J65:J70,J74,J75:J78,J80,J83,J85:J87,J89:J90,J93,J95:J97,J99,J101:J102,J109,J117,J122:J123,J128:J133)</f>
         <v>0.62300464788680743</v>
       </c>
-      <c r="AB31">
+      <c r="AD31" s="2">
         <f>STDEV(K3:K4,K6:K7,K11,K13:K14,K20:K21,K24:K26,K29,K33,K35,K39,K51:K56,K62,K65:K70,K74,K75:K78,K80,K83,K85:K87,K89:K90,K93,K95:K97,K99,K101:K102,K109,K117,K122:K123,K128:K133)</f>
         <v>5.3679295144056498E-2</v>
       </c>
-      <c r="AC31">
+      <c r="AE31" s="2">
         <f>STDEV(L3:L4,L6:L7,L11,L13:L14,L20:L21,L24:L26,L29,L33,L35,L39,L51:L56,L62,L65:L70,L74,L75:L78,L80,L83,L85:L87,L89:L90,L93,L95:L97,L99,L101:L102,L109,L117,L122:L123,L128:L133)</f>
         <v>1.598600219403731</v>
       </c>
-      <c r="AD31">
+      <c r="AF31" s="2">
         <f>STDEV(M3:M4,M6:M7,M11,M13:M14,M20:M21,M24:M26,M29,M33,M35,M39,M51:M56,M62,M65:M70,M74,M75:M78,M80,M83,M85:M87,M89:M90,M93,M95:M97,M99,M101:M102,M109,M117,M122:M123,M128:M133)</f>
         <v>4.4050703879969039E-2</v>
       </c>
-      <c r="AE31">
+      <c r="AG31" s="2">
         <f>STDEV(N3:N4,N6:N7,N11,N13:N14,N20:N21,N24:N26,N29,N33,N35,N39,N51:N56,N62,N65:N70,N74,N75:N78,N80,N83,N85:N87,N89:N90,N93,N95:N97,N99,N101:N102,N109,N117,N122:N123,N128:N133)</f>
         <v>0.17732262047194189</v>
       </c>
-      <c r="AF31">
+      <c r="AH31" s="2">
         <f>STDEV(O3:O4,O6:O7,O11,O13:O14,O20:O21,O24:O26,O29,O33,O35,O39,O51:O56,O62,O65:O70,O74,O75:O78,O80,O83,O85:O87,O89:O90,O93,O95:O97,O99,O101:O102,O109,O117,O122:O123,O128:O133)</f>
         <v>10.472160107927772</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI31" s="2">
+        <f>STDEV(Q3:Q4,Q6:Q7,Q11,Q13:Q14,Q20:Q21,Q24:Q26,Q29,Q33,Q35,Q39,Q51:Q56,Q62,Q65:Q70,Q74,Q75:Q78,Q80,Q83,Q85:Q87,Q89:Q90,Q93,Q95:Q97,Q99,Q101:Q102,Q109,Q117,Q122:Q123,Q128:Q133)</f>
+        <v>3.4846348152951227E-2</v>
+      </c>
+      <c r="AJ31" s="2">
+        <f>STDEV(R3:R4,R6:R7,R11,R13:R14,R20:R21,R24:R26,R29,R33,R35,R39,R51:R56,R62,R65:R70,R74,R75:R78,R80,R83,R85:R87,R89:R90,R93,R95:R97,R99,R101:R102,R109,R117,R122:R123,R128:R133)</f>
+        <v>3.2365859488426074E-2</v>
+      </c>
+      <c r="AK31" s="2">
+        <f>STDEV(S3:S4,S6:S7,S11,S13:S14,S20:S21,S24:S26,S29,S33,S35,S39,S51:S56,S62,S65:S70,S74,S75:S78,S80,S83,S85:S87,S89:S90,S93,S95:S97,S99,S101:S102,S109,S117,S122:S123,S128:S133)</f>
+        <v>2.7099463003808489E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -3830,51 +4296,69 @@
         <f>IF(E32=4,"HH",IF(E32=1, "LL", IF(E32=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="2">
+        <v>0.35903079999999998</v>
+      </c>
+      <c r="R32" s="2">
+        <v>0.34964580000000001</v>
+      </c>
+      <c r="S32" s="2">
+        <v>0.34585880000000002</v>
+      </c>
+      <c r="T32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="R32">
+      <c r="U32">
         <v>3.62788341792145E-2</v>
       </c>
-      <c r="U32" t="s">
+      <c r="W32" t="s">
         <v>151</v>
       </c>
-      <c r="V32" t="s">
+      <c r="X32" t="s">
         <v>134</v>
       </c>
-      <c r="W32" t="s">
+      <c r="Y32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Z32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="AA32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AB32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AC32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AD32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AE32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AF32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AE32" t="s">
+      <c r="AG32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AF32" t="s">
+      <c r="AH32" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AI32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK32" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
@@ -3924,61 +4408,83 @@
         <f>IF(E33=4,"HH",IF(E33=1, "LL", IF(E33=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="2">
+        <v>0.43504569999999998</v>
+      </c>
+      <c r="R33" s="2">
+        <v>0.419404</v>
+      </c>
+      <c r="S33" s="2">
+        <v>0.40610849999999998</v>
+      </c>
+      <c r="T33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="R33">
+      <c r="U33">
         <v>3.8166569712270802E-2</v>
       </c>
-      <c r="U33" t="s">
+      <c r="W33" t="s">
         <v>152</v>
       </c>
-      <c r="V33" t="s">
+      <c r="X33" t="s">
         <v>133</v>
       </c>
-      <c r="W33">
+      <c r="Y33" s="2">
         <f>STDEV(F2,F5,F8:F10,F15:F16,F18:F19,F22:F23,F27:F28,F30:F32,F34,F36:F38,F57:F61,F63:F64,F71:F73,F79,F81:F82,F84,F88,F91:F92,F94,F98,F100,F103:F108,F110:F116,F118:F121,F124:F127)</f>
         <v>5.0882715142944441</v>
       </c>
-      <c r="X33">
+      <c r="Z33" s="2">
         <f>STDEV(G2,G5,G8:G10,G15:G16,G18:G19,G22:G23,G27:G28,G30:G32,G34,G36:G38,G57:G61,G63:G64,G71:G73,G79,G81:G82,G84,G88,G91:G92,G94,G98,G100,G103:G108,G110:G116,G118:G121,G124:G127)</f>
         <v>4.821237747460243</v>
       </c>
-      <c r="Y33">
+      <c r="AA33" s="2">
         <f>STDEV(H2,H5,H8:H10,H15:H16,H18:H19,H22:H23,H27:H28,H30:H32,H34,H36:H38,H57:H61,H63:H64,H71:H73,H79,H81:H82,H84,H88,H91:H92,H94,H98,H100,H103:H108,H110:H116,H118:H121,H124:H127)</f>
         <v>6.3194619237673573</v>
       </c>
-      <c r="Z33">
+      <c r="AB33" s="2">
         <f>STDEV(I2,I5,I8:I10,I15:I16,I18:I19,I22:I23,I27:I28,I30:I32,I34,I36:I38,I57:I61,I63:I64,I71:I73,I79,I81:I82,I84,I88,I91:I92,I94,I98,I100,I103:I108,I110:I116,I118:I121,I124:I127)</f>
         <v>0.16286442259635489</v>
       </c>
-      <c r="AA33">
+      <c r="AC33" s="2">
         <f>STDEV(J2,J5,J8:J10,J15:J16,J18:J19,J22:J23,J27:J28,J30:J32,J34,J36:J38,J57:J61,J63:J64,J71:J73,J79,J81:J82,J84,J88,J91:J92,J94,J98,J100,J103:J108,J110:J116,J118:J121,J124:J127)</f>
         <v>0.76565643146142992</v>
       </c>
-      <c r="AB33">
+      <c r="AD33" s="2">
         <f>STDEV(K2,K5,K8:K10,K15:K16,K18:K19,K22:K23,K27:K28,K30:K32,K34,K36:K38,K57:K61,K63:K64,K71:K73,K79,K81:K82,K84,K88,K91:K92,K94,K98,K100,K103:K108,K110:K116,K118:K121,K124:K127)</f>
         <v>6.3881062639364661E-2</v>
       </c>
-      <c r="AC33">
+      <c r="AE33" s="2">
         <f>STDEV(L2,L5,L8:L10,L15:L16,L18:L19,L22:L23,L27:L28,L30:L32,L34,L36:L38,L57:L61,L63:L64,L71:L73,L79,L81:L82,L84,L88,L91:L92,L94,L98,L100,L103:L108,L110:L116,L118:L121,L124:L127)</f>
         <v>2.8950875098327269</v>
       </c>
-      <c r="AD33">
+      <c r="AF33" s="2">
         <f>STDEV(M2,M5,M8:M10,M15:M16,M18:M19,M22:M23,M27:M28,M30:M32,M34,M36:M38,M57:M61,M63:M64,M71:M73,M79,M81:M82,M84,M88,M91:M92,M94,M98,M100,M103:M108,M110:M116,M118:M121,M124:M127)</f>
         <v>6.1458066605247073E-2</v>
       </c>
-      <c r="AE33">
+      <c r="AG33" s="2">
         <f>STDEV(N2,N5,N8:N10,N15:N16,N18:N19,N22:N23,N27:N28,N30:N32,N34,N36:N38,N57:N61,N63:N64,N71:N73,N79,N81:N82,N84,N88,N91:N92,N94,N98,N100,N103:N108,N110:N116,N118:N121,N124:N127)</f>
         <v>0.20848733716909823</v>
       </c>
-      <c r="AF33">
+      <c r="AH33" s="2">
         <f>STDEV(O2,O5,O8:O10,O15:O16,O18:O19,O22:O23,O27:O28,O30:O32,O34,O36:O38,O57:O61,O63:O64,O71:O73,O79,O81:O82,O84,O88,O91:O92,O94,O98,O100,O103:O108,O110:O116,O118:O121,O124:O127)</f>
         <v>22.41415926415991</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AI33" s="2">
+        <f>STDEV(Q2,Q5,Q8:Q10,Q15:Q16,Q18:Q19,Q22:Q23,Q27:Q28,Q30:Q32,Q34,Q36:Q38,Q57:Q61,Q63:Q64,Q71:Q73,Q79,Q81:Q82,Q84,Q88,Q91:Q92,Q94,Q98,Q100,Q103:Q108,Q110:Q116,Q118:Q121,Q124:Q127)</f>
+        <v>4.7788112357791276E-2</v>
+      </c>
+      <c r="AJ33" s="2">
+        <f>STDEV(R2,R5,R8:R10,R15:R16,R18:R19,R22:R23,R27:R28,R30:R32,R34,R36:R38,R57:R61,R63:R64,R71:R73,R79,R81:R82,R84,R88,R91:R92,R94,R98,R100,R103:R108,R110:R116,R118:R121,R124:R127)</f>
+        <v>4.2862504383441025E-2</v>
+      </c>
+      <c r="AK33" s="2">
+        <f>STDEV(S2,S5,S8:S10,S15:S16,S18:S19,S22:S23,S27:S28,S30:S32,S34,S36:S38,S57:S61,S63:S64,S71:S73,S79,S81:S82,S84,S88,S91:S92,S94,S98,S100,S103:S108,S110:S116,S118:S121,S124:S127)</f>
+        <v>3.9144441933056752E-2</v>
+      </c>
+      <c r="AM33" s="2"/>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
@@ -4028,15 +4534,24 @@
         <f>IF(E34=4,"HH",IF(E34=1, "LL", IF(E34=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="2">
+        <v>0.35721429999999998</v>
+      </c>
+      <c r="R34" s="2">
+        <v>0.34996969999999999</v>
+      </c>
+      <c r="S34" s="2">
+        <v>0.34865249999999998</v>
+      </c>
+      <c r="T34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="R34">
+      <c r="U34">
         <v>2.8217292763456098E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
@@ -4086,15 +4601,24 @@
         <f>IF(E35=4,"HH",IF(E35=1, "LL", IF(E35=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="2">
+        <v>0.44680409999999998</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0.42703770000000002</v>
+      </c>
+      <c r="S35" s="2">
+        <v>0.41187780000000002</v>
+      </c>
+      <c r="T35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="R35">
+      <c r="U35">
         <v>5.6331308719955099E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
@@ -4144,15 +4668,24 @@
         <f>IF(E36=4,"HH",IF(E36=1, "LL", IF(E36=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="2">
+        <v>0.34062209999999998</v>
+      </c>
+      <c r="R36" s="2">
+        <v>0.33234849999999999</v>
+      </c>
+      <c r="S36" s="2">
+        <v>0.33086660000000001</v>
+      </c>
+      <c r="T36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="R36">
+      <c r="U36">
         <v>2.89372873325262E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
@@ -4202,18 +4735,27 @@
         <f>IF(E37=4,"HH",IF(E37=1, "LL", IF(E37=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="2">
+        <v>0.36213040000000002</v>
+      </c>
+      <c r="R37" s="2">
+        <v>0.33751530000000002</v>
+      </c>
+      <c r="S37" s="2">
+        <v>0.33274039999999999</v>
+      </c>
+      <c r="T37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="R37">
+      <c r="U37">
         <v>5.4764537860071801E-2</v>
       </c>
-      <c r="U37" s="7" t="s">
+      <c r="W37" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
@@ -4263,42 +4805,51 @@
         <f>IF(E38=4,"HH",IF(E38=1, "LL", IF(E38=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="2">
+        <v>0.33802589999999999</v>
+      </c>
+      <c r="R38" s="2">
+        <v>0.32361899999999999</v>
+      </c>
+      <c r="S38" s="2">
+        <v>0.320326</v>
+      </c>
+      <c r="T38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="R38">
+      <c r="U38">
         <v>4.7950036081094098E-2</v>
       </c>
-      <c r="U38" s="4" t="s">
+      <c r="W38" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Y38" s="4">
+      <c r="AA38" s="4">
         <v>2015</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="AB38" t="s">
         <v>156</v>
       </c>
-      <c r="AA38" s="4" t="s">
+      <c r="AC38" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AB38">
+      <c r="AD38">
         <v>37764</v>
       </c>
-      <c r="AC38" t="s">
+      <c r="AE38" t="s">
         <v>159</v>
       </c>
-      <c r="AD38" s="4" t="s">
+      <c r="AF38" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AE38">
+      <c r="AG38">
         <v>155604</v>
       </c>
-      <c r="AF38" t="s">
+      <c r="AH38" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
@@ -4348,39 +4899,48 @@
         <f>IF(E39=4,"HH",IF(E39=1, "LL", IF(E39=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="2">
+        <v>0.434228</v>
+      </c>
+      <c r="R39" s="2">
+        <v>0.41405839999999999</v>
+      </c>
+      <c r="S39" s="2">
+        <v>0.39730529999999997</v>
+      </c>
+      <c r="T39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="R39">
+      <c r="U39">
         <v>6.8084944889013094E-2</v>
       </c>
-      <c r="Y39" s="4">
+      <c r="AA39" s="4">
         <v>2016</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="AB39" t="s">
         <v>155</v>
       </c>
-      <c r="AA39" s="4" t="s">
+      <c r="AC39" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AB39">
+      <c r="AD39">
         <v>10858</v>
       </c>
-      <c r="AC39" t="s">
+      <c r="AE39" t="s">
         <v>159</v>
       </c>
-      <c r="AD39" s="4" t="s">
+      <c r="AF39" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="AE39">
+      <c r="AG39">
         <v>38519</v>
       </c>
-      <c r="AF39" t="s">
+      <c r="AH39" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>173</v>
       </c>
@@ -4403,15 +4963,15 @@
         <f>IF(E40=4,"HH",IF(E40=1, "LL", IF(E40=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q40" t="str">
+      <c r="T40" t="str">
         <f>A40</f>
         <v>Sensor 1</v>
       </c>
-      <c r="R40">
+      <c r="U40">
         <v>7.6873711775766906E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>174</v>
       </c>
@@ -4434,24 +4994,24 @@
         <f>IF(E41=4,"HH",IF(E41=1, "LL", IF(E41=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q41" t="str">
-        <f t="shared" ref="Q41:Q47" si="1">A41</f>
+      <c r="T41" t="str">
+        <f>A41</f>
         <v>Sensor 2</v>
       </c>
-      <c r="R41">
+      <c r="U41">
         <v>8.2396662160612505E-2</v>
       </c>
-      <c r="U41" s="4" t="s">
+      <c r="X41" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="Y41" s="4">
+      <c r="AB41" s="4">
         <v>2015</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="AC41" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>175</v>
       </c>
@@ -4474,27 +5034,27 @@
         <f>IF(E42=4,"HH",IF(E42=1, "LL", IF(E42=0, "NS", NA)))</f>
         <v>LL</v>
       </c>
-      <c r="Q42" t="str">
-        <f t="shared" si="1"/>
+      <c r="T42" t="str">
+        <f>A42</f>
         <v>Sensor 3</v>
       </c>
-      <c r="R42">
+      <c r="U42">
         <v>0.131071394534828</v>
       </c>
-      <c r="U42" s="4" t="s">
+      <c r="X42" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="Y42" s="4">
+      <c r="AB42" s="4">
         <v>2015</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="AC42" t="s">
         <v>163</v>
       </c>
-      <c r="AA42" s="4" t="s">
+      <c r="AD42" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>176</v>
       </c>
@@ -4517,31 +5077,31 @@
         <f>IF(E43=4,"HH",IF(E43=1, "LL", IF(E43=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q43" t="str">
-        <f t="shared" si="1"/>
+      <c r="T43" t="str">
+        <f>A43</f>
         <v>Sensor 5</v>
       </c>
-      <c r="R43">
+      <c r="U43">
         <v>3.7891107802974798E-2</v>
       </c>
-      <c r="U43" s="4" t="s">
+      <c r="X43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="Y43" s="4">
+      <c r="AB43" s="4">
         <v>2016</v>
       </c>
-      <c r="Z43" t="s">
+      <c r="AC43" t="s">
         <v>162</v>
       </c>
-      <c r="AA43" s="4">
+      <c r="AD43" s="4">
         <v>2015</v>
       </c>
-      <c r="AB43" s="2">
-        <f>(AB38/AE38)*100</f>
+      <c r="AE43" s="2">
+        <f>(AD38/AG38)*100</f>
         <v>24.269298989743191</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>177</v>
       </c>
@@ -4564,31 +5124,31 @@
         <f>IF(E44=4,"HH",IF(E44=1, "LL", IF(E44=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q44" t="str">
-        <f t="shared" si="1"/>
+      <c r="T44" t="str">
+        <f>A44</f>
         <v>Sensor 10</v>
       </c>
-      <c r="R44">
+      <c r="U44">
         <v>8.3386949030910904E-3</v>
       </c>
-      <c r="U44" s="4" t="s">
+      <c r="X44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="Y44" s="4">
+      <c r="AB44" s="4">
         <v>2016</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="AC44" t="s">
         <v>164</v>
       </c>
-      <c r="AA44" s="4">
+      <c r="AD44" s="4">
         <v>2016</v>
       </c>
-      <c r="AB44" s="2">
-        <f>(AB39/AE39)*100</f>
+      <c r="AE44" s="2">
+        <f>(AD39/AG39)*100</f>
         <v>28.188686102962173</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>178</v>
       </c>
@@ -4611,15 +5171,15 @@
         <f>IF(E45=4,"HH",IF(E45=1, "LL", IF(E45=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q45" t="str">
-        <f t="shared" si="1"/>
+      <c r="T45" t="str">
+        <f>A45</f>
         <v>Sensor 14</v>
       </c>
-      <c r="R45">
+      <c r="U45">
         <v>9.6592788843009002E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>179</v>
       </c>
@@ -4642,18 +5202,18 @@
         <f>IF(E46=4,"HH",IF(E46=1, "LL", IF(E46=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q46" t="str">
-        <f t="shared" si="1"/>
+      <c r="T46" t="str">
+        <f>A46</f>
         <v>Sensor 15</v>
       </c>
-      <c r="R46">
+      <c r="U46">
         <v>6.6200698679809294E-2</v>
       </c>
-      <c r="U46" t="s">
+      <c r="X46" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>180</v>
       </c>
@@ -4676,15 +5236,15 @@
         <f>IF(E47=4,"HH",IF(E47=1, "LL", IF(E47=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-      <c r="Q47" t="str">
-        <f t="shared" si="1"/>
+      <c r="T47" t="str">
+        <f>A47</f>
         <v>Sensor 19</v>
       </c>
-      <c r="R47">
+      <c r="U47">
         <v>4.6254226941092901E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>181</v>
       </c>
@@ -4707,15 +5267,15 @@
         <f>IF(E48=4,"HH",IF(E48=1, "LL", IF(E48=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-      <c r="Q48" t="str">
+      <c r="T48" t="str">
         <f>A48</f>
         <v>Sensor 20</v>
       </c>
-      <c r="R48">
+      <c r="U48">
         <v>3.1987874231012597E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
@@ -4764,8 +5324,17 @@
       <c r="P50" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q50" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="S50" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>42</v>
       </c>
@@ -4815,8 +5384,17 @@
         <f>IF(E51=4,"HH",IF(E51=1, "LL", IF(E51=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q51" s="2">
+        <v>0.47477530000000001</v>
+      </c>
+      <c r="R51" s="2">
+        <v>0.43418859999999998</v>
+      </c>
+      <c r="S51" s="2">
+        <v>0.4005338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>43</v>
       </c>
@@ -4866,8 +5444,17 @@
         <f>IF(E52=4,"HH",IF(E52=1, "LL", IF(E52=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q52" s="2">
+        <v>0.39476729999999999</v>
+      </c>
+      <c r="R52" s="2">
+        <v>0.36799409999999999</v>
+      </c>
+      <c r="S52" s="2">
+        <v>0.34900680000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>44</v>
       </c>
@@ -4917,8 +5504,17 @@
         <f>IF(E53=4,"HH",IF(E53=1, "LL", IF(E53=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q53" s="2">
+        <v>0.42919210000000002</v>
+      </c>
+      <c r="R53" s="2">
+        <v>0.40166550000000001</v>
+      </c>
+      <c r="S53" s="2">
+        <v>0.38358229999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>45</v>
       </c>
@@ -4968,8 +5564,17 @@
         <f>IF(E54=4,"HH",IF(E54=1, "LL", IF(E54=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q54" s="2">
+        <v>0.44969189999999998</v>
+      </c>
+      <c r="R54" s="2">
+        <v>0.42281829999999998</v>
+      </c>
+      <c r="S54" s="2">
+        <v>0.40192220000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>46</v>
       </c>
@@ -5019,8 +5624,17 @@
         <f>IF(E55=4,"HH",IF(E55=1, "LL", IF(E55=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q55" s="2">
+        <v>0.4621112</v>
+      </c>
+      <c r="R55" s="2">
+        <v>0.42614580000000002</v>
+      </c>
+      <c r="S55" s="2">
+        <v>0.40017629999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>47</v>
       </c>
@@ -5070,8 +5684,17 @@
         <f>IF(E56=4,"HH",IF(E56=1, "LL", IF(E56=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q56" s="2">
+        <v>0.46131139999999998</v>
+      </c>
+      <c r="R56" s="2">
+        <v>0.4228846</v>
+      </c>
+      <c r="S56" s="2">
+        <v>0.39435340000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>48</v>
       </c>
@@ -5121,8 +5744,17 @@
         <f>IF(E57=4,"HH",IF(E57=1, "LL", IF(E57=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q57" s="2">
+        <v>0.35930220000000002</v>
+      </c>
+      <c r="R57" s="2">
+        <v>0.34101809999999999</v>
+      </c>
+      <c r="S57" s="2">
+        <v>0.32835989999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>49</v>
       </c>
@@ -5172,8 +5804,17 @@
         <f>IF(E58=4,"HH",IF(E58=1, "LL", IF(E58=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q58" s="2">
+        <v>0.35492259999999998</v>
+      </c>
+      <c r="R58" s="2">
+        <v>0.33488040000000002</v>
+      </c>
+      <c r="S58" s="2">
+        <v>0.32131799999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>50</v>
       </c>
@@ -5223,8 +5864,17 @@
         <f>IF(E59=4,"HH",IF(E59=1, "LL", IF(E59=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q59" s="2">
+        <v>0.3668245</v>
+      </c>
+      <c r="R59" s="2">
+        <v>0.3570797</v>
+      </c>
+      <c r="S59" s="2">
+        <v>0.3401016</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>51</v>
       </c>
@@ -5274,8 +5924,17 @@
         <f>IF(E60=4,"HH",IF(E60=1, "LL", IF(E60=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q60" s="2">
+        <v>0.34433570000000002</v>
+      </c>
+      <c r="R60" s="2">
+        <v>0.3358467</v>
+      </c>
+      <c r="S60" s="2">
+        <v>0.3187179</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>52</v>
       </c>
@@ -5325,8 +5984,17 @@
         <f>IF(E61=4,"HH",IF(E61=1, "LL", IF(E61=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q61" s="2">
+        <v>0.35163060000000002</v>
+      </c>
+      <c r="R61" s="2">
+        <v>0.33656130000000001</v>
+      </c>
+      <c r="S61" s="2">
+        <v>0.3216929</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>53</v>
       </c>
@@ -5376,8 +6044,17 @@
         <f>IF(E62=4,"HH",IF(E62=1, "LL", IF(E62=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q62" s="2">
+        <v>0.4663407</v>
+      </c>
+      <c r="R62" s="2">
+        <v>0.46056409999999998</v>
+      </c>
+      <c r="S62" s="2">
+        <v>0.42766270000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>54</v>
       </c>
@@ -5427,8 +6104,17 @@
         <f>IF(E63=4,"HH",IF(E63=1, "LL", IF(E63=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q63" s="2">
+        <v>0.36400369999999999</v>
+      </c>
+      <c r="R63" s="2">
+        <v>0.35430919999999999</v>
+      </c>
+      <c r="S63" s="2">
+        <v>0.3374315</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>55</v>
       </c>
@@ -5478,8 +6164,17 @@
         <f>IF(E64=4,"HH",IF(E64=1, "LL", IF(E64=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q64" s="2">
+        <v>0.44874019999999998</v>
+      </c>
+      <c r="R64" s="2">
+        <v>0.43773960000000001</v>
+      </c>
+      <c r="S64" s="2">
+        <v>0.4081032</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>56</v>
       </c>
@@ -5529,8 +6224,17 @@
         <f>IF(E65=4,"HH",IF(E65=1, "LL", IF(E65=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q65" s="2">
+        <v>0.4490287</v>
+      </c>
+      <c r="R65" s="2">
+        <v>0.4392839</v>
+      </c>
+      <c r="S65" s="2">
+        <v>0.40668389999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>57</v>
       </c>
@@ -5580,8 +6284,17 @@
         <f>IF(E66=4,"HH",IF(E66=1, "LL", IF(E66=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q66" s="2">
+        <v>0.4433665</v>
+      </c>
+      <c r="R66" s="2">
+        <v>0.42051129999999998</v>
+      </c>
+      <c r="S66" s="2">
+        <v>0.39323590000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>58</v>
       </c>
@@ -5631,8 +6344,17 @@
         <f>IF(E67=4,"HH",IF(E67=1, "LL", IF(E67=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q67" s="2">
+        <v>0.45197229999999999</v>
+      </c>
+      <c r="R67" s="2">
+        <v>0.41163680000000002</v>
+      </c>
+      <c r="S67" s="2">
+        <v>0.38411020000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>59</v>
       </c>
@@ -5682,8 +6404,17 @@
         <f>IF(E68=4,"HH",IF(E68=1, "LL", IF(E68=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q68" s="2">
+        <v>0.4369133</v>
+      </c>
+      <c r="R68" s="2">
+        <v>0.39592480000000002</v>
+      </c>
+      <c r="S68" s="2">
+        <v>0.3656857</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>60</v>
       </c>
@@ -5733,8 +6464,17 @@
         <f>IF(E69=4,"HH",IF(E69=1, "LL", IF(E69=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q69" s="2">
+        <v>0.46218229999999999</v>
+      </c>
+      <c r="R69" s="2">
+        <v>0.4257145</v>
+      </c>
+      <c r="S69" s="2">
+        <v>0.3987907</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>61</v>
       </c>
@@ -5784,8 +6524,17 @@
         <f>IF(E70=4,"HH",IF(E70=1, "LL", IF(E70=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q70" s="2">
+        <v>0.44555319999999998</v>
+      </c>
+      <c r="R70" s="2">
+        <v>0.40099829999999997</v>
+      </c>
+      <c r="S70" s="2">
+        <v>0.37693759999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>62</v>
       </c>
@@ -5835,8 +6584,17 @@
         <f>IF(E71=4,"HH",IF(E71=1, "LL", IF(E71=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q71" s="2">
+        <v>0.29922260000000001</v>
+      </c>
+      <c r="R71" s="2">
+        <v>0.28539199999999998</v>
+      </c>
+      <c r="S71" s="2">
+        <v>0.28806759999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>63</v>
       </c>
@@ -5886,8 +6644,17 @@
         <f>IF(E72=4,"HH",IF(E72=1, "LL", IF(E72=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q72" s="2">
+        <v>0.34706169999999997</v>
+      </c>
+      <c r="R72" s="2">
+        <v>0.3399818</v>
+      </c>
+      <c r="S72" s="2">
+        <v>0.33672999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>64</v>
       </c>
@@ -5937,8 +6704,17 @@
         <f>IF(E73=4,"HH",IF(E73=1, "LL", IF(E73=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q73" s="2">
+        <v>0.33687810000000001</v>
+      </c>
+      <c r="R73" s="2">
+        <v>0.33280300000000002</v>
+      </c>
+      <c r="S73" s="2">
+        <v>0.33025090000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>65</v>
       </c>
@@ -5988,8 +6764,17 @@
         <f>IF(E74=4,"HH",IF(E74=1, "LL", IF(E74=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q74" s="2">
+        <v>0.4209157</v>
+      </c>
+      <c r="R74" s="2">
+        <v>0.40103430000000001</v>
+      </c>
+      <c r="S74" s="2">
+        <v>0.38827390000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>66</v>
       </c>
@@ -6039,8 +6824,17 @@
         <f>IF(E75=4,"HH",IF(E75=1, "LL", IF(E75=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q75" s="2">
+        <v>0.43194860000000002</v>
+      </c>
+      <c r="R75" s="2">
+        <v>0.4092269</v>
+      </c>
+      <c r="S75" s="2">
+        <v>0.40202349999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>67</v>
       </c>
@@ -6090,8 +6884,17 @@
         <f>IF(E76=4,"HH",IF(E76=1, "LL", IF(E76=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q76" s="2">
+        <v>0.36420730000000001</v>
+      </c>
+      <c r="R76" s="2">
+        <v>0.34000380000000002</v>
+      </c>
+      <c r="S76" s="2">
+        <v>0.33691660000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>68</v>
       </c>
@@ -6141,8 +6944,17 @@
         <f>IF(E77=4,"HH",IF(E77=1, "LL", IF(E77=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q77" s="2">
+        <v>0.42015429999999998</v>
+      </c>
+      <c r="R77" s="2">
+        <v>0.39944960000000002</v>
+      </c>
+      <c r="S77" s="2">
+        <v>0.38368439999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>69</v>
       </c>
@@ -6192,8 +7004,17 @@
         <f>IF(E78=4,"HH",IF(E78=1, "LL", IF(E78=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q78" s="2">
+        <v>0.3661952</v>
+      </c>
+      <c r="R78" s="2">
+        <v>0.34359699999999999</v>
+      </c>
+      <c r="S78" s="2">
+        <v>0.3412096</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>70</v>
       </c>
@@ -6243,8 +7064,17 @@
         <f>IF(E79=4,"HH",IF(E79=1, "LL", IF(E79=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q79" s="2">
+        <v>0.35030610000000001</v>
+      </c>
+      <c r="R79" s="2">
+        <v>0.34511960000000003</v>
+      </c>
+      <c r="S79" s="2">
+        <v>0.34203250000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>71</v>
       </c>
@@ -6294,8 +7124,17 @@
         <f>IF(E80=4,"HH",IF(E80=1, "LL", IF(E80=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q80" s="2">
+        <v>0.41965710000000001</v>
+      </c>
+      <c r="R80" s="2">
+        <v>0.40450930000000002</v>
+      </c>
+      <c r="S80" s="2">
+        <v>0.3926134</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>72</v>
       </c>
@@ -6345,8 +7184,17 @@
         <f>IF(E81=4,"HH",IF(E81=1, "LL", IF(E81=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q81" s="2">
+        <v>0.34266160000000001</v>
+      </c>
+      <c r="R81" s="2">
+        <v>0.3307657</v>
+      </c>
+      <c r="S81" s="2">
+        <v>0.33125969999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>73</v>
       </c>
@@ -6396,8 +7244,17 @@
         <f>IF(E82=4,"HH",IF(E82=1, "LL", IF(E82=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q82" s="2">
+        <v>0.35137360000000001</v>
+      </c>
+      <c r="R82" s="2">
+        <v>0.34927429999999998</v>
+      </c>
+      <c r="S82" s="2">
+        <v>0.34491110000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>74</v>
       </c>
@@ -6447,8 +7304,17 @@
         <f>IF(E83=4,"HH",IF(E83=1, "LL", IF(E83=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q83" s="2">
+        <v>0.39843600000000001</v>
+      </c>
+      <c r="R83" s="2">
+        <v>0.37151580000000001</v>
+      </c>
+      <c r="S83" s="2">
+        <v>0.35768519999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>75</v>
       </c>
@@ -6498,8 +7364,17 @@
         <f>IF(E84=4,"HH",IF(E84=1, "LL", IF(E84=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q84" s="2">
+        <v>0.43363429999999997</v>
+      </c>
+      <c r="R84" s="2">
+        <v>0.42890070000000002</v>
+      </c>
+      <c r="S84" s="2">
+        <v>0.42392000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>76</v>
       </c>
@@ -6549,8 +7424,17 @@
         <f>IF(E85=4,"HH",IF(E85=1, "LL", IF(E85=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q85" s="2">
+        <v>0.38877010000000001</v>
+      </c>
+      <c r="R85" s="2">
+        <v>0.36699520000000002</v>
+      </c>
+      <c r="S85" s="2">
+        <v>0.36538989999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>77</v>
       </c>
@@ -6600,8 +7484,17 @@
         <f>IF(E86=4,"HH",IF(E86=1, "LL", IF(E86=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q86" s="2">
+        <v>0.4044896</v>
+      </c>
+      <c r="R86" s="2">
+        <v>0.38156220000000002</v>
+      </c>
+      <c r="S86" s="2">
+        <v>0.37645800000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>78</v>
       </c>
@@ -6651,8 +7544,17 @@
         <f>IF(E87=4,"HH",IF(E87=1, "LL", IF(E87=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q87" s="2">
+        <v>0.42620190000000002</v>
+      </c>
+      <c r="R87" s="2">
+        <v>0.40615580000000001</v>
+      </c>
+      <c r="S87" s="2">
+        <v>0.39220169999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>79</v>
       </c>
@@ -6702,8 +7604,17 @@
         <f>IF(E88=4,"HH",IF(E88=1, "LL", IF(E88=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q88" s="2">
+        <v>0.30688320000000002</v>
+      </c>
+      <c r="R88" s="2">
+        <v>0.30144979999999999</v>
+      </c>
+      <c r="S88" s="2">
+        <v>0.30404300000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>80</v>
       </c>
@@ -6753,8 +7664,17 @@
         <f>IF(E89=4,"HH",IF(E89=1, "LL", IF(E89=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q89" s="2">
+        <v>0.41015049999999997</v>
+      </c>
+      <c r="R89" s="2">
+        <v>0.3884167</v>
+      </c>
+      <c r="S89" s="2">
+        <v>0.37417450000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>81</v>
       </c>
@@ -6804,8 +7724,17 @@
         <f>IF(E90=4,"HH",IF(E90=1, "LL", IF(E90=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q90" s="2">
+        <v>0.43450670000000002</v>
+      </c>
+      <c r="R90" s="2">
+        <v>0.4065163</v>
+      </c>
+      <c r="S90" s="2">
+        <v>0.39108039999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>82</v>
       </c>
@@ -6855,8 +7784,17 @@
         <f>IF(E91=4,"HH",IF(E91=1, "LL", IF(E91=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q91" s="2">
+        <v>0.28306110000000001</v>
+      </c>
+      <c r="R91" s="2">
+        <v>0.26540239999999998</v>
+      </c>
+      <c r="S91" s="2">
+        <v>0.26655499999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>83</v>
       </c>
@@ -6906,8 +7844,17 @@
         <f>IF(E92=4,"HH",IF(E92=1, "LL", IF(E92=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q92" s="2">
+        <v>0.3347021</v>
+      </c>
+      <c r="R92" s="2">
+        <v>0.32753979999999999</v>
+      </c>
+      <c r="S92" s="2">
+        <v>0.32457619999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>84</v>
       </c>
@@ -6957,8 +7904,17 @@
         <f>IF(E93=4,"HH",IF(E93=1, "LL", IF(E93=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q93" s="2">
+        <v>0.35266900000000001</v>
+      </c>
+      <c r="R93" s="2">
+        <v>0.33369310000000002</v>
+      </c>
+      <c r="S93" s="2">
+        <v>0.33101760000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>85</v>
       </c>
@@ -7008,8 +7964,17 @@
         <f>IF(E94=4,"HH",IF(E94=1, "LL", IF(E94=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q94" s="2">
+        <v>0.34811029999999998</v>
+      </c>
+      <c r="R94" s="2">
+        <v>0.34263569999999999</v>
+      </c>
+      <c r="S94" s="2">
+        <v>0.33740809999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>86</v>
       </c>
@@ -7059,8 +8024,17 @@
         <f>IF(E95=4,"HH",IF(E95=1, "LL", IF(E95=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q95" s="2">
+        <v>0.3836367</v>
+      </c>
+      <c r="R95" s="2">
+        <v>0.3599271</v>
+      </c>
+      <c r="S95" s="2">
+        <v>0.34696090000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>87</v>
       </c>
@@ -7110,8 +8084,17 @@
         <f>IF(E96=4,"HH",IF(E96=1, "LL", IF(E96=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q96" s="2">
+        <v>0.36232330000000001</v>
+      </c>
+      <c r="R96" s="2">
+        <v>0.34408830000000001</v>
+      </c>
+      <c r="S96" s="2">
+        <v>0.34182439999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>88</v>
       </c>
@@ -7161,8 +8144,17 @@
         <f>IF(E97=4,"HH",IF(E97=1, "LL", IF(E97=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q97" s="2">
+        <v>0.40377150000000001</v>
+      </c>
+      <c r="R97" s="2">
+        <v>0.38442520000000002</v>
+      </c>
+      <c r="S97" s="2">
+        <v>0.37195299999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>89</v>
       </c>
@@ -7212,8 +8204,17 @@
         <f>IF(E98=4,"HH",IF(E98=1, "LL", IF(E98=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q98" s="2">
+        <v>0.33350760000000002</v>
+      </c>
+      <c r="R98" s="2">
+        <v>0.32432840000000002</v>
+      </c>
+      <c r="S98" s="2">
+        <v>0.31959470000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>90</v>
       </c>
@@ -7263,8 +8264,17 @@
         <f>IF(E99=4,"HH",IF(E99=1, "LL", IF(E99=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q99" s="2">
+        <v>0.40986489999999998</v>
+      </c>
+      <c r="R99" s="2">
+        <v>0.39125949999999998</v>
+      </c>
+      <c r="S99" s="2">
+        <v>0.38059850000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>91</v>
       </c>
@@ -7314,8 +8324,17 @@
         <f>IF(E100=4,"HH",IF(E100=1, "LL", IF(E100=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q100" s="2">
+        <v>0.46183419999999997</v>
+      </c>
+      <c r="R100" s="2">
+        <v>0.42771049999999999</v>
+      </c>
+      <c r="S100" s="2">
+        <v>0.41379759999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>92</v>
       </c>
@@ -7365,8 +8384,17 @@
         <f>IF(E101=4,"HH",IF(E101=1, "LL", IF(E101=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q101" s="2">
+        <v>0.40232050000000003</v>
+      </c>
+      <c r="R101" s="2">
+        <v>0.38639059999999997</v>
+      </c>
+      <c r="S101" s="2">
+        <v>0.37239539999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>93</v>
       </c>
@@ -7416,8 +8444,17 @@
         <f>IF(E102=4,"HH",IF(E102=1, "LL", IF(E102=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q102" s="2">
+        <v>0.36417739999999998</v>
+      </c>
+      <c r="R102" s="2">
+        <v>0.34837099999999999</v>
+      </c>
+      <c r="S102" s="2">
+        <v>0.34721849999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>94</v>
       </c>
@@ -7467,8 +8504,17 @@
         <f>IF(E103=4,"HH",IF(E103=1, "LL", IF(E103=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q103" s="2">
+        <v>0.42390549999999999</v>
+      </c>
+      <c r="R103" s="2">
+        <v>0.40031939999999999</v>
+      </c>
+      <c r="S103" s="2">
+        <v>0.39537990000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>95</v>
       </c>
@@ -7518,8 +8564,17 @@
         <f>IF(E104=4,"HH",IF(E104=1, "LL", IF(E104=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q104" s="2">
+        <v>0.47243950000000001</v>
+      </c>
+      <c r="R104" s="2">
+        <v>0.44259670000000001</v>
+      </c>
+      <c r="S104" s="2">
+        <v>0.43098890000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>96</v>
       </c>
@@ -7569,8 +8624,17 @@
         <f>IF(E105=4,"HH",IF(E105=1, "LL", IF(E105=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q105" s="2">
+        <v>0.444519</v>
+      </c>
+      <c r="R105" s="2">
+        <v>0.44241979999999997</v>
+      </c>
+      <c r="S105" s="2">
+        <v>0.43525750000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>97</v>
       </c>
@@ -7620,8 +8684,17 @@
         <f>IF(E106=4,"HH",IF(E106=1, "LL", IF(E106=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q106" s="2">
+        <v>0.45722309999999999</v>
+      </c>
+      <c r="R106" s="2">
+        <v>0.43207279999999998</v>
+      </c>
+      <c r="S106" s="2">
+        <v>0.40926879999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>98</v>
       </c>
@@ -7671,8 +8744,17 @@
         <f>IF(E107=4,"HH",IF(E107=1, "LL", IF(E107=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q107" s="2">
+        <v>0.45173350000000001</v>
+      </c>
+      <c r="R107" s="2">
+        <v>0.42370190000000002</v>
+      </c>
+      <c r="S107" s="2">
+        <v>0.41579870000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>99</v>
       </c>
@@ -7722,8 +8804,17 @@
         <f>IF(E108=4,"HH",IF(E108=1, "LL", IF(E108=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q108" s="2">
+        <v>0.32803159999999998</v>
+      </c>
+      <c r="R108" s="2">
+        <v>0.3196756</v>
+      </c>
+      <c r="S108" s="2">
+        <v>0.31741170000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>100</v>
       </c>
@@ -7773,8 +8864,17 @@
         <f>IF(E109=4,"HH",IF(E109=1, "LL", IF(E109=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q109" s="2">
+        <v>0.40424909999999997</v>
+      </c>
+      <c r="R109" s="2">
+        <v>0.390295</v>
+      </c>
+      <c r="S109" s="2">
+        <v>0.38103350000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>101</v>
       </c>
@@ -7824,8 +8924,17 @@
         <f>IF(E110=4,"HH",IF(E110=1, "LL", IF(E110=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q110" s="2">
+        <v>0.33140360000000002</v>
+      </c>
+      <c r="R110" s="2">
+        <v>0.32111299999999998</v>
+      </c>
+      <c r="S110" s="2">
+        <v>0.3228007</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>102</v>
       </c>
@@ -7875,8 +8984,17 @@
         <f>IF(E111=4,"HH",IF(E111=1, "LL", IF(E111=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q111" s="2">
+        <v>0.334727</v>
+      </c>
+      <c r="R111" s="2">
+        <v>0.32550659999999998</v>
+      </c>
+      <c r="S111" s="2">
+        <v>0.32110230000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>103</v>
       </c>
@@ -7926,8 +9044,17 @@
         <f>IF(E112=4,"HH",IF(E112=1, "LL", IF(E112=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q112" s="2">
+        <v>0.4287049</v>
+      </c>
+      <c r="R112" s="2">
+        <v>0.42006080000000001</v>
+      </c>
+      <c r="S112" s="2">
+        <v>0.40713579999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>104</v>
       </c>
@@ -7977,8 +9104,17 @@
         <f>IF(E113=4,"HH",IF(E113=1, "LL", IF(E113=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q113" s="2">
+        <v>0.34188059999999998</v>
+      </c>
+      <c r="R113" s="2">
+        <v>0.33615899999999999</v>
+      </c>
+      <c r="S113" s="2">
+        <v>0.33183699999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>105</v>
       </c>
@@ -8028,8 +9164,17 @@
         <f>IF(E114=4,"HH",IF(E114=1, "LL", IF(E114=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q114" s="2">
+        <v>0.3418292</v>
+      </c>
+      <c r="R114" s="2">
+        <v>0.33779530000000002</v>
+      </c>
+      <c r="S114" s="2">
+        <v>0.33306160000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>106</v>
       </c>
@@ -8079,8 +9224,17 @@
         <f>IF(E115=4,"HH",IF(E115=1, "LL", IF(E115=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q115" s="2">
+        <v>0.33099630000000002</v>
+      </c>
+      <c r="R115" s="2">
+        <v>0.3166718</v>
+      </c>
+      <c r="S115" s="2">
+        <v>0.31745390000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>107</v>
       </c>
@@ -8130,8 +9284,17 @@
         <f>IF(E116=4,"HH",IF(E116=1, "LL", IF(E116=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q116" s="2">
+        <v>0.32829710000000001</v>
+      </c>
+      <c r="R116" s="2">
+        <v>0.32014690000000001</v>
+      </c>
+      <c r="S116" s="2">
+        <v>0.31586599999999998</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>108</v>
       </c>
@@ -8181,8 +9344,17 @@
         <f>IF(E117=4,"HH",IF(E117=1, "LL", IF(E117=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q117" s="2">
+        <v>0.40415319999999999</v>
+      </c>
+      <c r="R117" s="2">
+        <v>0.37743880000000002</v>
+      </c>
+      <c r="S117" s="2">
+        <v>0.36344359999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>109</v>
       </c>
@@ -8232,8 +9404,17 @@
         <f>IF(E118=4,"HH",IF(E118=1, "LL", IF(E118=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q118" s="2">
+        <v>0.3360552</v>
+      </c>
+      <c r="R118" s="2">
+        <v>0.31428030000000001</v>
+      </c>
+      <c r="S118" s="2">
+        <v>0.31341590000000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>110</v>
       </c>
@@ -8283,8 +9464,17 @@
         <f>IF(E119=4,"HH",IF(E119=1, "LL", IF(E119=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q119" s="2">
+        <v>0.33661609999999997</v>
+      </c>
+      <c r="R119" s="2">
+        <v>0.33077099999999998</v>
+      </c>
+      <c r="S119" s="2">
+        <v>0.32389689999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>111</v>
       </c>
@@ -8334,8 +9524,17 @@
         <f>IF(E120=4,"HH",IF(E120=1, "LL", IF(E120=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q120" s="2">
+        <v>0.3436186</v>
+      </c>
+      <c r="R120" s="2">
+        <v>0.33863789999999999</v>
+      </c>
+      <c r="S120" s="2">
+        <v>0.33081700000000003</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>112</v>
       </c>
@@ -8385,8 +9584,17 @@
         <f>IF(E121=4,"HH",IF(E121=1, "LL", IF(E121=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q121" s="2">
+        <v>0.35896270000000002</v>
+      </c>
+      <c r="R121" s="2">
+        <v>0.35480529999999999</v>
+      </c>
+      <c r="S121" s="2">
+        <v>0.34826049999999997</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>113</v>
       </c>
@@ -8436,8 +9644,17 @@
         <f>IF(E122=4,"HH",IF(E122=1, "LL", IF(E122=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q122" s="2">
+        <v>0.43089290000000002</v>
+      </c>
+      <c r="R122" s="2">
+        <v>0.41574509999999998</v>
+      </c>
+      <c r="S122" s="2">
+        <v>0.4039315</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>114</v>
       </c>
@@ -8487,8 +9704,17 @@
         <f>IF(E123=4,"HH",IF(E123=1, "LL", IF(E123=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q123" s="2">
+        <v>0.4198788</v>
+      </c>
+      <c r="R123" s="2">
+        <v>0.39345259999999999</v>
+      </c>
+      <c r="S123" s="2">
+        <v>0.37628780000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>115</v>
       </c>
@@ -8538,8 +9764,17 @@
         <f>IF(E124=4,"HH",IF(E124=1, "LL", IF(E124=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q124" s="2">
+        <v>0.41889939999999998</v>
+      </c>
+      <c r="R124" s="2">
+        <v>0.39189679999999999</v>
+      </c>
+      <c r="S124" s="2">
+        <v>0.37786049999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>116</v>
       </c>
@@ -8589,8 +9824,17 @@
         <f>IF(E125=4,"HH",IF(E125=1, "LL", IF(E125=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q125" s="2">
+        <v>0.35281669999999998</v>
+      </c>
+      <c r="R125" s="2">
+        <v>0.34359630000000002</v>
+      </c>
+      <c r="S125" s="2">
+        <v>0.33771010000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>117</v>
       </c>
@@ -8640,8 +9884,17 @@
         <f>IF(E126=4,"HH",IF(E126=1, "LL", IF(E126=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q126" s="2">
+        <v>0.30290260000000002</v>
+      </c>
+      <c r="R126" s="2">
+        <v>0.2910066</v>
+      </c>
+      <c r="S126" s="2">
+        <v>0.287055</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>118</v>
       </c>
@@ -8691,8 +9944,17 @@
         <f>IF(E127=4,"HH",IF(E127=1, "LL", IF(E127=0, "NS", NA)))</f>
         <v>NS</v>
       </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q127" s="2">
+        <v>0.3204708</v>
+      </c>
+      <c r="R127" s="2">
+        <v>0.31195010000000001</v>
+      </c>
+      <c r="S127" s="2">
+        <v>0.30614619999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>119</v>
       </c>
@@ -8742,8 +10004,17 @@
         <f>IF(E128=4,"HH",IF(E128=1, "LL", IF(E128=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q128" s="2">
+        <v>0.38837310000000003</v>
+      </c>
+      <c r="R128" s="2">
+        <v>0.36873860000000003</v>
+      </c>
+      <c r="S128" s="2">
+        <v>0.35494920000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>120</v>
       </c>
@@ -8793,8 +10064,17 @@
         <f>IF(E129=4,"HH",IF(E129=1, "LL", IF(E129=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q129" s="2">
+        <v>0.4058561</v>
+      </c>
+      <c r="R129" s="2">
+        <v>0.38589230000000002</v>
+      </c>
+      <c r="S129" s="2">
+        <v>0.37337890000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>121</v>
       </c>
@@ -8844,8 +10124,17 @@
         <f>IF(E130=4,"HH",IF(E130=1, "LL", IF(E130=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q130" s="2">
+        <v>0.4373379</v>
+      </c>
+      <c r="R130" s="2">
+        <v>0.43132809999999999</v>
+      </c>
+      <c r="S130" s="2">
+        <v>0.42239589999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>122</v>
       </c>
@@ -8895,8 +10184,17 @@
         <f>IF(E131=4,"HH",IF(E131=1, "LL", IF(E131=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q131" s="2">
+        <v>0.42167320000000003</v>
+      </c>
+      <c r="R131" s="2">
+        <v>0.40697820000000001</v>
+      </c>
+      <c r="S131" s="2">
+        <v>0.39417669999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>123</v>
       </c>
@@ -8946,8 +10244,17 @@
         <f>IF(E132=4,"HH",IF(E132=1, "LL", IF(E132=0, "NS", NA)))</f>
         <v>HH</v>
       </c>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q132" s="2">
+        <v>0.38844790000000001</v>
+      </c>
+      <c r="R132" s="2">
+        <v>0.36770199999999997</v>
+      </c>
+      <c r="S132" s="2">
+        <v>0.35625889999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>124</v>
       </c>
@@ -8996,6 +10303,15 @@
       <c r="P133" t="str">
         <f>IF(E133=4,"HH",IF(E133=1, "LL", IF(E133=0, "NS", NA)))</f>
         <v>HH</v>
+      </c>
+      <c r="Q133" s="2">
+        <v>0.37714769999999997</v>
+      </c>
+      <c r="R133" s="2">
+        <v>0.35471409999999998</v>
+      </c>
+      <c r="S133" s="2">
+        <v>0.34882790000000002</v>
       </c>
     </row>
   </sheetData>
@@ -9009,7 +10325,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="F1" sqref="F1:F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>